<commit_message>
Update read time for event emails
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donnagalletta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55118904-A40B-4566-A795-08534EE7D8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7907713-D386-410B-BC2D-E1A2C88B81A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="740" windowWidth="29920" windowHeight="17700" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -179,12 +179,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{C85A22D2-5413-4932-95A0-6343FF53898D}">
+      <text>
+        <t>Donna Galletta:
+Filter via: 
+Aggregate Report</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
   <si>
     <t>img-id</t>
   </si>
@@ -231,6 +238,9 @@
     <t>read-under-2s</t>
   </si>
   <si>
+    <t>Litmus-tacking-id</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALL BRANDS - WEBINAR - JUL 25 - Financial Literacy - Invite </t>
   </si>
   <si>
@@ -240,21 +250,51 @@
     <t>Event</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18380262/analytics</t>
+  </si>
+  <si>
     <t>Media</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/358386/emails/18105943/analytics</t>
+  </si>
+  <si>
     <t>WEBINAR - WAG - JUL Super health check seminar INVITE</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18300323/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18300326/analytics</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEMINAR - AUG (TAS) Retirement Seminar &amp; webinars (CBUS &amp; MS) INVITE </t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18452986/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18452988/analytics</t>
+  </si>
+  <si>
     <t>WEBINAR - JUL Transition to Retirement strategy (TTR) INVITE</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18452760/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18452759/analytics</t>
+  </si>
+  <si>
     <t>SEMINAR - AUG (CAN) Retirement Seminar &amp; webinars (CBUS &amp; MS) INVITE</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18485780/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18485781/analytics</t>
+  </si>
+  <si>
     <t>EOFY Performance - Accum</t>
   </si>
   <si>
@@ -273,6 +313,12 @@
     <t>WEBINAR - WAG - JUL How much is enough? INVITE</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18529297/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18529296/analytics</t>
+  </si>
+  <si>
     <t>CBUS - Corporate insurance SEN (AME)</t>
   </si>
   <si>
@@ -282,7 +328,19 @@
     <t>WEBINAR - JUL EOFY Investment Update INVITE</t>
   </si>
   <si>
+    <t>https://litmus.com/folders/324180/emails/18619780/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18619775/analytics</t>
+  </si>
+  <si>
     <t>WEBINAR - WAG - AUG Choosing the right investment option INVITE</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18679502/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/18679501/analytics</t>
   </si>
   <si>
     <t>SEMINAR - AUG (TAS) Retirement Seminar &amp; webinars (CBUS &amp; MS) REMINDER</t>
@@ -574,7 +632,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -712,6 +770,21 @@
     </xf>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -720,7 +793,26 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="3" xr:uid="{770A8CE4-86FC-45BF-95B8-E1D8E67E3936}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1194,32 +1286,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="B1:O26" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16" headerRowBorderDxfId="14" tableBorderDxfId="15">
-  <autoFilter ref="B1:O26" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="B1:P26" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16">
+  <autoFilter ref="B1:P26" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J2">
     <sortCondition ref="C1:C2"/>
   </sortState>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{592A3136-8A60-4650-9DF6-CD74A33464B1}" name="name" dataDxfId="13" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" xr3:uid="{1F194343-9489-4FF7-8BA8-8FE4AD211F8B}" name="date" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="2" xr3:uid="{613F8D1F-C5D7-46FB-834A-5183617D5BF8}" name="brand" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{39913B7C-CBB3-470C-8F4E-6888A201DA8B}" name="type" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{0D81733F-25B3-4A7C-B3C0-DFE06A90464F}" name="unique-sends" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{274A7B85-7FDE-4D40-8515-C885EF39314B}" name="unique-opens" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{C860F744-163F-46E0-BC1A-15DDD6121358}" name="unique-clicks" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{A71DAAD5-121C-41AC-A08E-BF363CF89DFE}" name="unsub" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{3E23A808-3FEF-4D90-BACE-62A3345A0868}" name="unsub-pc" dataDxfId="5">
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{592A3136-8A60-4650-9DF6-CD74A33464B1}" name="name" dataDxfId="14" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" xr3:uid="{1F194343-9489-4FF7-8BA8-8FE4AD211F8B}" name="date" dataDxfId="13" dataCellStyle="Hyperlink"/>
+    <tableColumn id="2" xr3:uid="{613F8D1F-C5D7-46FB-834A-5183617D5BF8}" name="brand" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{39913B7C-CBB3-470C-8F4E-6888A201DA8B}" name="type" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{0D81733F-25B3-4A7C-B3C0-DFE06A90464F}" name="unique-sends" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{274A7B85-7FDE-4D40-8515-C885EF39314B}" name="unique-opens" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{C860F744-163F-46E0-BC1A-15DDD6121358}" name="unique-clicks" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{A71DAAD5-121C-41AC-A08E-BF363CF89DFE}" name="unsub" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{3E23A808-3FEF-4D90-BACE-62A3345A0868}" name="unsub-pc" dataDxfId="6">
       <calculatedColumnFormula>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E7D2EFD0-301C-4002-8501-CE02665F086E}" name="unique-opens-pc" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{E7D2EFD0-301C-4002-8501-CE02665F086E}" name="unique-opens-pc" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FE8ED384-E8DC-43C9-9628-C6A9E5DFA5BE}" name="unique-clicks-pc" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{FE8ED384-E8DC-43C9-9628-C6A9E5DFA5BE}" name="unique-clicks-pc" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{3CA46112-C95F-E64B-A58D-81BDEBF2FDC4}" name="read-over-8s" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{985DCAD1-25BF-804E-9E49-5E19FC44B93C}" name="read-under-8s" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{986830C2-C7E6-C645-8ACD-C78E1B2E462F}" name="read-under-2s" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{3CA46112-C95F-E64B-A58D-81BDEBF2FDC4}" name="read-over-8s" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{985DCAD1-25BF-804E-9E49-5E19FC44B93C}" name="read-under-8s" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{986830C2-C7E6-C645-8ACD-C78E1B2E462F}" name="read-under-2s" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{D273CFB9-324F-4CB2-B1BA-58EEE2D8C50F}" name="Litmus-tacking-id" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1542,11 +1635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23CF1A7-A843-E143-B142-84B9EDCB7AA1}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <pane ySplit="1" topLeftCell="E17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="32.1" customHeight="1"/>
@@ -1566,11 +1659,11 @@
     <col min="13" max="13" width="17.125" style="24" customWidth="1"/>
     <col min="14" max="14" width="14.625" style="23" customWidth="1"/>
     <col min="15" max="15" width="15.375" style="14" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="14" customWidth="1"/>
+    <col min="16" max="16" width="52" style="55" customWidth="1"/>
     <col min="17" max="16384" width="10.875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="32.1" customHeight="1">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="32.1" customHeight="1">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -1616,22 +1709,25 @@
       <c r="O1" s="30" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="52" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" s="10" customFormat="1" ht="32.1" customHeight="1">
+    <row r="2" spans="1:16" s="10" customFormat="1" ht="32.1" customHeight="1">
       <c r="A2" s="45">
         <v>31</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="25">
         <v>45839</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="7">
         <v>9564</v>
@@ -1658,30 +1754,33 @@
         <v>0.52279381012128812</v>
       </c>
       <c r="M2" s="9">
-        <v>0</v>
+        <v>61.9</v>
       </c>
       <c r="N2" s="9">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="O2" s="9">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="P2" s="56" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="32.1" customHeight="1">
+    <row r="3" spans="1:16" ht="32.1" customHeight="1">
       <c r="A3" s="19">
         <v>31</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="18">
         <v>45839</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="15">
         <v>230</v>
@@ -1708,30 +1807,33 @@
         <v>0</v>
       </c>
       <c r="M3" s="9">
-        <v>0</v>
+        <v>83.3</v>
       </c>
       <c r="N3" s="9">
-        <v>0</v>
+        <v>16.7</v>
       </c>
       <c r="O3" s="9">
         <v>0</v>
       </c>
+      <c r="P3" s="53" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" ht="32.1" customHeight="1">
+    <row r="4" spans="1:16" ht="32.1" customHeight="1">
       <c r="A4" s="46">
         <v>31</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" s="18">
         <v>45846</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="15">
         <v>8314</v>
@@ -1758,30 +1860,33 @@
         <v>1.5155159971133028</v>
       </c>
       <c r="M4" s="9">
-        <v>0</v>
+        <v>78.8</v>
       </c>
       <c r="N4" s="9">
-        <v>0</v>
+        <v>14.1</v>
       </c>
       <c r="O4" s="9">
-        <v>0</v>
+        <v>7.1</v>
+      </c>
+      <c r="P4" s="53" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="32.1" customHeight="1">
+    <row r="5" spans="1:16" ht="32.1" customHeight="1">
       <c r="A5" s="19">
         <v>31</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" s="18">
         <v>45846</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>17</v>
       </c>
       <c r="F5" s="15">
         <v>465</v>
@@ -1808,30 +1913,33 @@
         <v>2.3655913978494625</v>
       </c>
       <c r="M5" s="9">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N5" s="9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O5" s="9">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="P5" s="53" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="32.1" customHeight="1">
+    <row r="6" spans="1:16" ht="32.1" customHeight="1">
       <c r="A6" s="46">
         <v>30</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C6" s="18">
         <v>45846</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="15">
         <v>2085</v>
@@ -1858,30 +1966,33 @@
         <v>4.8920863309352516</v>
       </c>
       <c r="M6" s="9">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="N6" s="9">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="O6" s="9">
-        <v>0</v>
+        <v>8.9</v>
+      </c>
+      <c r="P6" s="53" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="32.1" customHeight="1">
+    <row r="7" spans="1:16" ht="32.1" customHeight="1">
       <c r="A7" s="13">
         <v>30</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C7" s="18">
         <v>45846</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>17</v>
       </c>
       <c r="F7" s="11">
         <v>217</v>
@@ -1908,30 +2019,33 @@
         <v>5.9907834101382482</v>
       </c>
       <c r="M7" s="9">
-        <v>0</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="N7" s="9">
-        <v>0</v>
+        <v>19.2</v>
       </c>
       <c r="O7" s="9">
-        <v>0</v>
+        <v>7.7</v>
+      </c>
+      <c r="P7" s="53" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="32.1" customHeight="1">
+    <row r="8" spans="1:16" ht="32.1" customHeight="1">
       <c r="A8" s="46">
         <v>30</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C8" s="18">
         <v>45846</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="15">
         <v>8369</v>
@@ -1958,30 +2072,33 @@
         <v>2.8079818377344963</v>
       </c>
       <c r="M8" s="9">
-        <v>0</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="N8" s="9">
-        <v>0</v>
+        <v>14.6</v>
       </c>
       <c r="O8" s="9">
-        <v>0</v>
+        <v>11.8</v>
+      </c>
+      <c r="P8" s="53" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="32.1" customHeight="1">
+    <row r="9" spans="1:16" ht="32.1" customHeight="1">
       <c r="A9" s="13">
         <v>30</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C9" s="18">
         <v>45846</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>17</v>
       </c>
       <c r="F9" s="11">
         <v>1253</v>
@@ -2008,30 +2125,33 @@
         <v>3.6711891460494814</v>
       </c>
       <c r="M9" s="9">
-        <v>0</v>
+        <v>66.7</v>
       </c>
       <c r="N9" s="9">
-        <v>0</v>
+        <v>25.3</v>
       </c>
       <c r="O9" s="9">
-        <v>0</v>
+        <v>8.1</v>
+      </c>
+      <c r="P9" s="53" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="32.1" customHeight="1">
+    <row r="10" spans="1:16" ht="32.1" customHeight="1">
       <c r="A10" s="46">
         <v>30</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C10" s="18">
         <v>45848</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="15">
         <v>1542</v>
@@ -2058,30 +2178,33 @@
         <v>2.8534370946822309</v>
       </c>
       <c r="M10" s="9">
-        <v>0</v>
+        <v>75.8</v>
       </c>
       <c r="N10" s="9">
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="O10" s="9">
-        <v>0</v>
+        <v>11.1</v>
+      </c>
+      <c r="P10" s="53" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32.1" customHeight="1">
+    <row r="11" spans="1:16" ht="32.1" customHeight="1">
       <c r="A11" s="13">
         <v>30</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C11" s="18">
         <v>45848</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="26" t="s">
         <v>18</v>
-      </c>
-      <c r="E11" s="26" t="s">
-        <v>17</v>
       </c>
       <c r="F11" s="11">
         <v>182</v>
@@ -2108,30 +2231,33 @@
         <v>2.197802197802198</v>
       </c>
       <c r="M11" s="9">
-        <v>0</v>
+        <v>66.7</v>
       </c>
       <c r="N11" s="9">
-        <v>0</v>
+        <v>14.8</v>
       </c>
       <c r="O11" s="9">
-        <v>0</v>
+        <v>18.5</v>
+      </c>
+      <c r="P11" s="53" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="32.1" customHeight="1">
+    <row r="12" spans="1:16" ht="32.1" customHeight="1">
       <c r="A12" s="46">
         <v>61</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C12" s="18">
         <v>45852</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F12" s="15">
         <v>320093</v>
@@ -2166,22 +2292,23 @@
       <c r="O12" s="9">
         <v>14.3</v>
       </c>
+      <c r="P12" s="54"/>
     </row>
-    <row r="13" spans="1:15" ht="32.1" customHeight="1">
+    <row r="13" spans="1:16" ht="32.1" customHeight="1">
       <c r="A13" s="19">
         <v>5</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C13" s="18">
         <v>45852</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F13" s="15">
         <v>28154</v>
@@ -2216,22 +2343,23 @@
       <c r="O13" s="19">
         <v>17.2</v>
       </c>
+      <c r="P13" s="54"/>
     </row>
-    <row r="14" spans="1:15" ht="32.1" customHeight="1">
+    <row r="14" spans="1:16" ht="32.1" customHeight="1">
       <c r="A14" s="47">
         <v>62</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C14" s="18">
         <v>45852</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F14" s="11">
         <v>20052</v>
@@ -2266,22 +2394,23 @@
       <c r="O14" s="13">
         <v>11.6</v>
       </c>
+      <c r="P14" s="54"/>
     </row>
-    <row r="15" spans="1:15" ht="32.1" customHeight="1">
+    <row r="15" spans="1:16" ht="32.1" customHeight="1">
       <c r="A15" s="13">
         <v>63</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C15" s="18">
         <v>45852</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F15" s="11">
         <v>6012</v>
@@ -2316,22 +2445,23 @@
       <c r="O15" s="13">
         <v>9</v>
       </c>
+      <c r="P15" s="54"/>
     </row>
-    <row r="16" spans="1:15" ht="32.1" customHeight="1">
+    <row r="16" spans="1:16" ht="32.1" customHeight="1">
       <c r="A16" s="46">
         <v>31</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C16" s="18">
         <v>45853</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F16" s="15">
         <v>6597</v>
@@ -2358,30 +2488,33 @@
         <v>2.6678793390935271</v>
       </c>
       <c r="M16" s="9">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="N16" s="9">
-        <v>0</v>
+        <v>23.4</v>
       </c>
       <c r="O16" s="9">
-        <v>0</v>
+        <v>12.6</v>
+      </c>
+      <c r="P16" s="53" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="32.1" customHeight="1">
+    <row r="17" spans="1:16" ht="32.1" customHeight="1">
       <c r="A17" s="19">
         <v>31</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C17" s="18">
         <v>45853</v>
       </c>
       <c r="D17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="F17" s="15">
         <v>432</v>
@@ -2408,30 +2541,33 @@
         <v>4.8611111111111116</v>
       </c>
       <c r="M17" s="9">
-        <v>0</v>
+        <v>51.2</v>
       </c>
       <c r="N17" s="9">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="O17" s="9">
-        <v>0</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P17" s="53" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="32.1" customHeight="1">
+    <row r="18" spans="1:16" ht="32.1" customHeight="1">
       <c r="A18" s="46">
         <v>77</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C18" s="18">
         <v>45860</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F18" s="11">
         <v>28</v>
@@ -2466,22 +2602,23 @@
       <c r="O18" s="19">
         <v>30</v>
       </c>
+      <c r="P18" s="54"/>
     </row>
-    <row r="19" spans="1:15" ht="32.1" customHeight="1">
+    <row r="19" spans="1:16" ht="32.1" customHeight="1">
       <c r="A19" s="13">
         <v>31</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C19" s="18">
         <v>45861</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19" s="15">
         <v>52075</v>
@@ -2508,30 +2645,33 @@
         <v>1.6361017762842056</v>
       </c>
       <c r="M19" s="9">
-        <v>0</v>
+        <v>63.7</v>
       </c>
       <c r="N19" s="9">
-        <v>0</v>
+        <v>22.8</v>
       </c>
       <c r="O19" s="9">
-        <v>0</v>
+        <v>13.6</v>
+      </c>
+      <c r="P19" s="53" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="32.1" customHeight="1">
+    <row r="20" spans="1:16" ht="32.1" customHeight="1">
       <c r="A20" s="47">
         <v>31</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C20" s="18">
         <v>45861</v>
       </c>
       <c r="D20" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="F20" s="11">
         <v>8068</v>
@@ -2558,30 +2698,33 @@
         <v>3.3341596430342091</v>
       </c>
       <c r="M20" s="9">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="N20" s="9">
-        <v>0</v>
+        <v>22.4</v>
       </c>
       <c r="O20" s="9">
-        <v>0</v>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="P20" s="53" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="32.1" customHeight="1">
+    <row r="21" spans="1:16" ht="32.1" customHeight="1">
       <c r="A21" s="13">
         <v>31</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C21" s="18">
         <v>45867</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" s="15">
         <v>8974</v>
@@ -2608,30 +2751,33 @@
         <v>1.8386449743704034</v>
       </c>
       <c r="M21" s="9">
-        <v>0</v>
+        <v>61.8</v>
       </c>
       <c r="N21" s="9">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="O21" s="9">
-        <v>0</v>
+        <v>19.100000000000001</v>
+      </c>
+      <c r="P21" s="53" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="32.1" customHeight="1">
+    <row r="22" spans="1:16" ht="32.1" customHeight="1">
       <c r="A22" s="47">
         <v>31</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="C22" s="18">
         <v>45867</v>
       </c>
       <c r="D22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="F22" s="15">
         <v>610</v>
@@ -2658,30 +2804,33 @@
         <v>1.9672131147540985</v>
       </c>
       <c r="M22" s="9">
-        <v>0</v>
+        <v>52.4</v>
       </c>
       <c r="N22" s="9">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="O22" s="9">
-        <v>0</v>
+        <v>33.299999999999997</v>
+      </c>
+      <c r="P22" s="53" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="32.1" customHeight="1">
+    <row r="23" spans="1:16" ht="32.1" customHeight="1">
       <c r="A23" s="19">
         <v>30</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C23" s="18">
         <v>45867</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" s="15">
         <v>1628</v>
@@ -2716,22 +2865,23 @@
       <c r="O23" s="9">
         <v>0</v>
       </c>
+      <c r="P23" s="54"/>
     </row>
-    <row r="24" spans="1:15" ht="32.1" customHeight="1">
+    <row r="24" spans="1:16" ht="32.1" customHeight="1">
       <c r="A24" s="46">
         <v>30</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C24" s="18">
         <v>45867</v>
       </c>
       <c r="D24" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="F24" s="15">
         <v>188</v>
@@ -2766,22 +2916,23 @@
       <c r="O24" s="9">
         <v>0</v>
       </c>
+      <c r="P24" s="54"/>
     </row>
-    <row r="25" spans="1:15" ht="32.1" customHeight="1">
+    <row r="25" spans="1:16" ht="32.1" customHeight="1">
       <c r="A25" s="19">
         <v>30</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C25" s="18">
         <v>45867</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F25" s="15">
         <v>1217</v>
@@ -2816,22 +2967,23 @@
       <c r="O25" s="9">
         <v>0</v>
       </c>
+      <c r="P25" s="54"/>
     </row>
-    <row r="26" spans="1:15" ht="32.1" customHeight="1">
+    <row r="26" spans="1:16" ht="32.1" customHeight="1">
       <c r="A26" s="47">
         <v>30</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C26" s="18">
         <v>45867</v>
       </c>
       <c r="D26" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="17" t="s">
         <v>18</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="F26" s="11">
         <v>155</v>
@@ -2866,6 +3018,7 @@
       <c r="O26" s="9">
         <v>0</v>
       </c>
+      <c r="P26" s="54"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2894,11 +3047,27 @@
     <hyperlink ref="B25" r:id="rId23" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{9AB33328-4010-F843-B550-8D7E64EC2CD1}"/>
     <hyperlink ref="B26" r:id="rId24" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{1CD36E2E-A888-B64A-A43F-52462AF0D631}"/>
     <hyperlink ref="B3" r:id="rId25" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/541e1d3f-d064-4e8c-ad26-a2f26946d5ec" xr:uid="{BFA6D6B9-0F92-4A98-BC01-3F66ECBAF652}"/>
+    <hyperlink ref="P3" r:id="rId26" xr:uid="{51BBEF75-8B33-4A54-A5A5-C3E2872BA63D}"/>
+    <hyperlink ref="P2" r:id="rId27" xr:uid="{9B91B3EB-9AC1-4462-A67A-81961D7FCB79}"/>
+    <hyperlink ref="P4" r:id="rId28" xr:uid="{1077084C-D29E-4ABC-BD53-A05F91719125}"/>
+    <hyperlink ref="P5" r:id="rId29" xr:uid="{E82B6BA4-E16F-492E-BCD8-911C556EA12C}"/>
+    <hyperlink ref="P6" r:id="rId30" xr:uid="{6184ED25-1DF9-49D3-AC87-98D010A3B3E0}"/>
+    <hyperlink ref="P7" r:id="rId31" xr:uid="{23489B88-1AF7-440D-82A5-D2C99B402CE1}"/>
+    <hyperlink ref="P8" r:id="rId32" xr:uid="{29D38B7B-0EEB-4F1D-BD67-2FE0B692C886}"/>
+    <hyperlink ref="P9" r:id="rId33" xr:uid="{E529B59E-BC39-41D7-A6B8-B76C65B02964}"/>
+    <hyperlink ref="P10" r:id="rId34" xr:uid="{75D776C4-686E-4764-A0CE-7978746739AA}"/>
+    <hyperlink ref="P11" r:id="rId35" xr:uid="{18534669-D2F7-4C45-BE71-B06E441E98C4}"/>
+    <hyperlink ref="P16" r:id="rId36" xr:uid="{4456DFDD-02ED-4178-A1B2-7A56262C79A7}"/>
+    <hyperlink ref="P17" r:id="rId37" xr:uid="{85BEFFFA-77A3-49CF-94D8-7F3EBFED1A80}"/>
+    <hyperlink ref="P19" r:id="rId38" xr:uid="{9D50E18A-27F4-4E22-95C5-F200362F77FE}"/>
+    <hyperlink ref="P20" r:id="rId39" xr:uid="{49F0C4D7-6B49-48CB-9B69-3680BAAED979}"/>
+    <hyperlink ref="P21" r:id="rId40" xr:uid="{669F8622-A0EA-44FE-8AAA-EAB6EE53AEB9}"/>
+    <hyperlink ref="P22" r:id="rId41" xr:uid="{3EC869FD-833C-4252-AFF2-954077725E77}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId26"/>
+  <legacyDrawing r:id="rId42"/>
   <tableParts count="1">
-    <tablePart r:id="rId27"/>
+    <tablePart r:id="rId43"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update SIS statement data
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donnagalletta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2D73BDE-82AD-41B7-8B8C-B8CD114EC9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BB36386-98D9-4901-88EF-44DC29C9AF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="740" windowWidth="29920" windowHeight="17700" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -205,17 +205,35 @@
     </comment>
     <comment ref="O1" authorId="0" shapeId="0" xr:uid="{392D3804-56EC-4160-B43F-7901312E770F}">
       <text>
-        <t>Donna Galletta:
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Donna Galletta:
 Engagement Score (%)=Open Rate (%)+Click Rate (%)−2×Unsub Rate (%)</t>
+        </r>
       </text>
     </comment>
     <comment ref="P1" authorId="0" shapeId="0" xr:uid="{E6510ECF-D05E-4F7D-9FA1-A4B9CE20D238}">
       <text>
-        <t>Donna Galletta:
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Donna Galletta:
 Traffic Light Logic:
 🟢 Green = Engagement Score ≥ 80
 🟡 Yellow = Engagement Score ≥ 50 and &lt; 80
 🔴 Red = Engagement Score &lt; 50</t>
+        </r>
       </text>
     </comment>
     <comment ref="T1" authorId="0" shapeId="0" xr:uid="{C85A22D2-5413-4932-95A0-6343FF53898D}">
@@ -255,7 +273,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="163">
   <si>
     <t>img-id</t>
   </si>
@@ -735,6 +753,15 @@
   </si>
   <si>
     <t>Abandoned  Cart MJOL</t>
+  </si>
+  <si>
+    <t>Cbus - 2025 Statements - SIS</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/416254/emails/19097350/analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cbus - 2025 Statements - SIS - Microsoft </t>
   </si>
 </sst>
 </file>
@@ -2069,8 +2096,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="B1:T142" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="24" tableBorderDxfId="25">
-  <autoFilter ref="B1:T142" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="B1:T144" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="24" tableBorderDxfId="25">
+  <autoFilter ref="B1:T144" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:T94">
     <sortCondition descending="1" ref="F1:F94"/>
   </sortState>
@@ -2438,11 +2465,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23CF1A7-A843-E143-B142-84B9EDCB7AA1}">
-  <dimension ref="A1:T142"/>
+  <dimension ref="A1:T144"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="I2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <pane ySplit="1" topLeftCell="H139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q144" sqref="Q144:S144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="32.1" customHeight="1"/>
@@ -11969,6 +11996,142 @@
         <v>0</v>
       </c>
       <c r="T142" s="45"/>
+    </row>
+    <row r="143" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A143" s="62">
+        <v>74</v>
+      </c>
+      <c r="B143" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C143" s="61">
+        <v>45922</v>
+      </c>
+      <c r="D143" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="E143" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="F143" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G143" s="14">
+        <v>10911</v>
+      </c>
+      <c r="H143" s="30">
+        <v>8376</v>
+      </c>
+      <c r="I143" s="34">
+        <v>4289</v>
+      </c>
+      <c r="J143" s="17">
+        <v>8</v>
+      </c>
+      <c r="K143" s="41">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>7.3320502245440386E-2</v>
+      </c>
+      <c r="L143" s="27">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>76.766565850976079</v>
+      </c>
+      <c r="M143" s="48">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>39.308954266336727</v>
+      </c>
+      <c r="N143" s="48">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>51.205826170009551</v>
+      </c>
+      <c r="O143" s="48">
+        <f>MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*100 + (Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]]*100) - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>115.92887911282193</v>
+      </c>
+      <c r="P143" s="48" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;=30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;=60,"🟡","🟢"))</f>
+        <v>🟢</v>
+      </c>
+      <c r="Q143" s="15">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="R143" s="17">
+        <v>17.2</v>
+      </c>
+      <c r="S143" s="17">
+        <v>13.5</v>
+      </c>
+      <c r="T143" s="49" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A144" s="62">
+        <v>74</v>
+      </c>
+      <c r="B144" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C144" s="61">
+        <v>45922</v>
+      </c>
+      <c r="D144" s="76" t="s">
+        <v>21</v>
+      </c>
+      <c r="E144" s="78" t="s">
+        <v>40</v>
+      </c>
+      <c r="F144" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G144" s="10">
+        <v>3043</v>
+      </c>
+      <c r="H144" s="31">
+        <v>2080</v>
+      </c>
+      <c r="I144" s="35">
+        <v>1053</v>
+      </c>
+      <c r="J144" s="12">
+        <v>0</v>
+      </c>
+      <c r="K144" s="42">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L144" s="7">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>68.353598422609267</v>
+      </c>
+      <c r="M144" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>34.60400920144594</v>
+      </c>
+      <c r="N144" s="48">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>50.625</v>
+      </c>
+      <c r="O144" s="48">
+        <f>MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*100 + (Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]]*100) - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>102.95760762405521</v>
+      </c>
+      <c r="P144" s="48" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;=30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;=60,"🟡","🟢"))</f>
+        <v>🟢</v>
+      </c>
+      <c r="Q144" s="15">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="R144" s="17">
+        <v>17.2</v>
+      </c>
+      <c r="S144" s="17">
+        <v>13.5</v>
+      </c>
+      <c r="T144" s="44" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B46:B51">
@@ -12197,17 +12360,41 @@
     <hyperlink ref="B140" r:id="rId203" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" xr:uid="{FC6E80E8-E09B-4E1C-800C-92FA7943F72B}"/>
     <hyperlink ref="B141:B142" r:id="rId204" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" display="Abandoned  Cart MJOL" xr:uid="{89E7B679-7362-475D-98BE-25F1829C350A}"/>
     <hyperlink ref="T89" r:id="rId205" xr:uid="{1ABD2676-EB8A-4847-847A-4104CD4746DF}"/>
+    <hyperlink ref="B143" r:id="rId206" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bd610eaf-020d-4ee0-8920-be3e08a37a25" xr:uid="{DEABCB06-B632-461D-84C6-F06A70FA9619}"/>
+    <hyperlink ref="B144" r:id="rId207" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3df19f42-c622-481a-a0cc-b64ea8f94164" display="Cbus - 2025 Statements - SIS" xr:uid="{8C7106E8-B2C7-4073-98E2-6BD22D598D4F}"/>
+    <hyperlink ref="T144" r:id="rId208" xr:uid="{46704411-4366-4503-871A-63C62D6F5CDF}"/>
+    <hyperlink ref="T143" r:id="rId209" xr:uid="{35617BE4-D51B-4C42-BCBC-A3326810417E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId206"/>
+  <legacyDrawing r:id="rId210"/>
   <tableParts count="2">
-    <tablePart r:id="rId207"/>
-    <tablePart r:id="rId208"/>
+    <tablePart r:id="rId211"/>
+    <tablePart r:id="rId212"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005CAB1339F159CD428AD0F5BA99C368F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f0c74bf1a42c2d75d8315edd8b34847e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0eeac73-9918-465e-bdd8-785547fbc2d9" xmlns:ns3="d777fa6b-bca0-4864-8d50-ac77b155e846" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e574cbbd1e27f27e000ab280241298b2" ns2:_="" ns3:_="">
     <xsd:import namespace="c0eeac73-9918-465e-bdd8-785547fbc2d9"/>
@@ -12442,28 +12629,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCFB8158-C1A2-453A-A951-1338C1FD9481}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12471,7 +12638,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCFB8158-C1A2-453A-A951-1338C1FD9481}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
update data and table to fit laptop screen
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donnagalletta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4252A4E7-9534-4518-B181-8F4CBEDEDA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A63BDDF-EC72-4B77-8816-0B1431584528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="320" yWindow="740" windowWidth="29920" windowHeight="17700" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -205,21 +205,39 @@
     </comment>
     <comment ref="O1" authorId="0" shapeId="0" xr:uid="{392D3804-56EC-4160-B43F-7901312E770F}">
       <text>
-        <t xml:space="preserve">Engagement Score (%) =
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">Engagement Score (%) =
 (Open Rate (%) × 0.5) + (Click Rate (%) × 0.5) − 2 × Unsub Rate (%)
 &gt;Open Rate: Accounts for 50% of the score. Campaigns with more opens get a higher score.
 &gt;Click Rate: Also accounts for 50% of the score. Campaigns with very few clicks will see their score reduced, even if open rates are high.
 &gt;Unsubscribe Rate: Each unsubscribe counts double, so campaigns with higher unsubscribes are penalised more.
 Rewards campaigns that not only get opened but also encourage engagement.
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="P1" authorId="0" shapeId="0" xr:uid="{E6510ECF-D05E-4F7D-9FA1-A4B9CE20D238}">
       <text>
-        <t xml:space="preserve">🟢 Green: Score ≥ 40 (really strong engagement, opens + clicks significant)
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">🟢 Green: Score ≥ 40 (really strong engagement, opens + clicks significant)
 🟡 Yellow: Score ≥ 30 and &lt; 40 (moderate engagement)
 🔴 Red: Score &lt; 30 (low engagement, clicks too low)
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="T1" authorId="0" shapeId="0" xr:uid="{C85A22D2-5413-4932-95A0-6343FF53898D}">
@@ -259,7 +277,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="166">
   <si>
     <t>img-id</t>
   </si>
@@ -748,6 +766,15 @@
   </si>
   <si>
     <t xml:space="preserve">Cbus - 2025 Statements - SIS - Microsoft </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEBINAR - OCT 25 - Super Health Check seminar </t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/358386/emails/19028939/analytics</t>
+  </si>
+  <si>
+    <t>https://litmus.com/folders/324180/emails/19332991/analytics</t>
   </si>
 </sst>
 </file>
@@ -2082,8 +2109,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="B1:T144" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="24" tableBorderDxfId="25">
-  <autoFilter ref="B1:T144" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="B1:T146" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26" headerRowBorderDxfId="24" tableBorderDxfId="25">
+  <autoFilter ref="B1:T146" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:T94">
     <sortCondition descending="1" ref="F1:F94"/>
   </sortState>
@@ -2454,11 +2481,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23CF1A7-A843-E143-B142-84B9EDCB7AA1}">
-  <dimension ref="A1:T144"/>
+  <dimension ref="A1:T146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="L139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T146" sqref="T146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="32.1" customHeight="1"/>
@@ -12549,6 +12576,148 @@
       </c>
       <c r="T144" s="44" t="s">
         <v>161</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A145" s="62">
+        <v>31</v>
+      </c>
+      <c r="B145" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="C145" s="61">
+        <v>45930</v>
+      </c>
+      <c r="D145" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E145" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F145" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G145" s="10">
+        <v>298</v>
+      </c>
+      <c r="H145" s="31">
+        <v>154</v>
+      </c>
+      <c r="I145" s="35">
+        <v>2</v>
+      </c>
+      <c r="J145" s="12">
+        <v>0</v>
+      </c>
+      <c r="K145" s="42">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L145" s="7">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>51.677852348993291</v>
+      </c>
+      <c r="M145" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>0.67114093959731547</v>
+      </c>
+      <c r="N145" s="48">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>1.2987012987012987</v>
+      </c>
+      <c r="O145" s="48">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>26.350164407008698</v>
+      </c>
+      <c r="P145" s="48" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🔴</v>
+      </c>
+      <c r="Q145" s="11">
+        <v>50</v>
+      </c>
+      <c r="R145" s="12">
+        <v>38.9</v>
+      </c>
+      <c r="S145" s="12">
+        <v>11.1</v>
+      </c>
+      <c r="T145" s="44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A146" s="62">
+        <v>31</v>
+      </c>
+      <c r="B146" s="57" t="s">
+        <v>163</v>
+      </c>
+      <c r="C146" s="61">
+        <v>45930</v>
+      </c>
+      <c r="D146" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E146" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G146" s="10">
+        <v>8785</v>
+      </c>
+      <c r="H146" s="31">
+        <v>4026</v>
+      </c>
+      <c r="I146" s="35">
+        <v>150</v>
+      </c>
+      <c r="J146" s="12">
+        <v>1</v>
+      </c>
+      <c r="K146" s="42">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>1.1383039271485488E-2</v>
+      </c>
+      <c r="L146" s="7">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>45.828116107000568</v>
+      </c>
+      <c r="M146" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>1.707455890722823</v>
+      </c>
+      <c r="N146" s="48">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>3.7257824143070044</v>
+      </c>
+      <c r="O146" s="48">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>24.150844382450686</v>
+      </c>
+      <c r="P146" s="48" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🔴</v>
+      </c>
+      <c r="Q146" s="11">
+        <v>79.5</v>
+      </c>
+      <c r="R146" s="12">
+        <v>14.4</v>
+      </c>
+      <c r="S146" s="12">
+        <v>6.1</v>
+      </c>
+      <c r="T146" s="44" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -12782,28 +12951,21 @@
     <hyperlink ref="B144" r:id="rId207" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3df19f42-c622-481a-a0cc-b64ea8f94164" display="Cbus - 2025 Statements - SIS" xr:uid="{8C7106E8-B2C7-4073-98E2-6BD22D598D4F}"/>
     <hyperlink ref="T144" r:id="rId208" xr:uid="{46704411-4366-4503-871A-63C62D6F5CDF}"/>
     <hyperlink ref="T143" r:id="rId209" xr:uid="{35617BE4-D51B-4C42-BCBC-A3326810417E}"/>
+    <hyperlink ref="B145" r:id="rId210" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df121502-9927-4eed-8a89-998f44dfe2cb" xr:uid="{4C7035C0-55DC-42DB-BC1A-1724968D036A}"/>
+    <hyperlink ref="B146" r:id="rId211" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df121502-9927-4eed-8a89-998f44dfe2cb" xr:uid="{D51BF1B3-CB4F-4C37-97E4-0E8A747D3371}"/>
+    <hyperlink ref="T145" r:id="rId212" xr:uid="{6D9DC780-9CDA-4D3F-B56F-0677CA3C5FB2}"/>
+    <hyperlink ref="T146" r:id="rId213" xr:uid="{E660BB65-5617-4FC2-B761-2C921DC44FB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId210"/>
+  <legacyDrawing r:id="rId214"/>
   <tableParts count="2">
-    <tablePart r:id="rId211"/>
-    <tablePart r:id="rId212"/>
+    <tablePart r:id="rId215"/>
+    <tablePart r:id="rId216"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005CAB1339F159CD428AD0F5BA99C368F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f0c74bf1a42c2d75d8315edd8b34847e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0eeac73-9918-465e-bdd8-785547fbc2d9" xmlns:ns3="d777fa6b-bca0-4864-8d50-ac77b155e846" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e574cbbd1e27f27e000ab280241298b2" ns2:_="" ns3:_="">
     <xsd:import namespace="c0eeac73-9918-465e-bdd8-785547fbc2d9"/>
@@ -13038,6 +13200,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -13048,11 +13221,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCFB8158-C1A2-453A-A951-1338C1FD9481}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCFB8158-C1A2-453A-A951-1338C1FD9481}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
remove unwanted items in row
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donnagalletta/email-gallery/cbus/pages/dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25146704-2006-C54B-A45B-6E313049CCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2CECDB8-EC7A-614B-A63C-449EF9069950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17700" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -294,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="244">
   <si>
     <t>img-id</t>
   </si>
@@ -1000,18 +1000,6 @@
   </si>
   <si>
     <t>https://litmus.com/folders/416254/emails/19414929/analytics</t>
-  </si>
-  <si>
-    <t>Media - 2025 Statements - RIE - Microsoft Version 1.0</t>
-  </si>
-  <si>
-    <t>Media - 2025 Statements - NON RIE - Microsoft Version 1.0</t>
-  </si>
-  <si>
-    <t>Tuesday, October 16, 2025</t>
-  </si>
-  <si>
-    <t>Tuesday, October 23, 2025</t>
   </si>
   <si>
     <t>Email - Cbus - 2025 Statements - 1.eDM [RIE - C]</t>
@@ -2932,11 +2920,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23CF1A7-A843-E143-B142-84B9EDCB7AA1}">
-  <dimension ref="A1:T238"/>
+  <dimension ref="A1:T224"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A222" sqref="A222"/>
+      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A225" sqref="A225:XFD240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18389,271 +18377,6 @@
       <c r="H224" s="12"/>
       <c r="I224" s="12"/>
       <c r="J224" s="12"/>
-    </row>
-    <row r="225" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A225" s="12"/>
-      <c r="B225" s="12"/>
-      <c r="C225" s="12"/>
-      <c r="D225" s="136"/>
-      <c r="E225" s="136"/>
-      <c r="F225" s="136"/>
-      <c r="G225" s="12"/>
-      <c r="H225" s="12"/>
-      <c r="I225" s="12"/>
-      <c r="J225" s="12"/>
-    </row>
-    <row r="226" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A226" s="12"/>
-      <c r="B226" s="12"/>
-      <c r="C226" s="12"/>
-      <c r="D226" s="136"/>
-      <c r="E226" s="136"/>
-      <c r="F226" s="136"/>
-      <c r="G226" s="12"/>
-      <c r="H226" s="12"/>
-      <c r="I226" s="12"/>
-      <c r="J226" s="12"/>
-    </row>
-    <row r="227" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A227" s="12"/>
-      <c r="B227" s="12"/>
-      <c r="C227" s="12"/>
-      <c r="D227" s="136"/>
-      <c r="E227" s="136"/>
-      <c r="F227" s="136"/>
-      <c r="G227" s="12"/>
-      <c r="H227" s="12"/>
-      <c r="I227" s="12"/>
-      <c r="J227" s="12"/>
-    </row>
-    <row r="228" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A228" s="12"/>
-      <c r="B228" s="12"/>
-      <c r="C228" s="12"/>
-      <c r="D228" s="136"/>
-      <c r="E228" s="136"/>
-      <c r="F228" s="136"/>
-      <c r="G228" s="12"/>
-      <c r="H228" s="12"/>
-      <c r="I228" s="12"/>
-      <c r="J228" s="12"/>
-    </row>
-    <row r="229" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A229" s="12"/>
-      <c r="B229" s="12"/>
-      <c r="C229" s="12"/>
-      <c r="D229" s="136"/>
-      <c r="E229" s="136"/>
-      <c r="F229" s="136"/>
-      <c r="G229" s="12"/>
-      <c r="H229" s="12"/>
-      <c r="I229" s="12"/>
-      <c r="J229" s="12"/>
-    </row>
-    <row r="230" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A230" s="12"/>
-      <c r="B230" s="12"/>
-      <c r="C230" s="12"/>
-      <c r="D230" s="136"/>
-      <c r="E230" s="136"/>
-      <c r="F230" s="136"/>
-      <c r="G230" s="12"/>
-      <c r="H230" s="12"/>
-      <c r="I230" s="12"/>
-      <c r="J230" s="12"/>
-    </row>
-    <row r="231" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A231" s="12"/>
-      <c r="B231" s="12"/>
-      <c r="C231" s="12"/>
-      <c r="D231" s="136"/>
-      <c r="E231" s="136"/>
-      <c r="F231" s="136"/>
-      <c r="G231" s="12"/>
-      <c r="H231" s="12"/>
-      <c r="I231" s="12"/>
-      <c r="J231" s="12"/>
-    </row>
-    <row r="232" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="12"/>
-      <c r="B232" s="12"/>
-      <c r="C232" s="12"/>
-      <c r="D232" s="136"/>
-      <c r="E232" s="136"/>
-      <c r="F232" s="136"/>
-      <c r="G232" s="12"/>
-      <c r="H232" s="12"/>
-      <c r="I232" s="12"/>
-      <c r="J232" s="12"/>
-    </row>
-    <row r="233" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A233" s="12"/>
-      <c r="B233" s="12"/>
-      <c r="C233" s="12"/>
-      <c r="D233" s="136"/>
-      <c r="E233" s="136"/>
-      <c r="F233" s="136"/>
-      <c r="G233" s="12"/>
-      <c r="H233" s="12"/>
-      <c r="I233" s="12"/>
-      <c r="J233" s="12"/>
-    </row>
-    <row r="234" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="81">
-        <v>76</v>
-      </c>
-      <c r="B234" s="100" t="s">
-        <v>235</v>
-      </c>
-      <c r="C234" s="100" t="s">
-        <v>214</v>
-      </c>
-      <c r="D234" s="101" t="s">
-        <v>28</v>
-      </c>
-      <c r="E234" s="101" t="s">
-        <v>68</v>
-      </c>
-      <c r="F234" s="101" t="s">
-        <v>26</v>
-      </c>
-      <c r="G234" s="100">
-        <v>5665</v>
-      </c>
-      <c r="H234" s="100">
-        <v>3502</v>
-      </c>
-      <c r="I234" s="100">
-        <v>1556</v>
-      </c>
-      <c r="J234" s="100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="235" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A235" s="81">
-        <v>76</v>
-      </c>
-      <c r="B235" s="100" t="s">
-        <v>236</v>
-      </c>
-      <c r="C235" s="100" t="s">
-        <v>222</v>
-      </c>
-      <c r="D235" s="101" t="s">
-        <v>28</v>
-      </c>
-      <c r="E235" s="101" t="s">
-        <v>68</v>
-      </c>
-      <c r="F235" s="101" t="s">
-        <v>26</v>
-      </c>
-      <c r="G235" s="100">
-        <v>4216</v>
-      </c>
-      <c r="H235" s="100">
-        <v>2280</v>
-      </c>
-      <c r="I235" s="100">
-        <v>880</v>
-      </c>
-      <c r="J235" s="100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="236" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A236" s="81">
-        <v>73</v>
-      </c>
-      <c r="B236" s="100" t="s">
-        <v>232</v>
-      </c>
-      <c r="C236" s="100" t="s">
-        <v>237</v>
-      </c>
-      <c r="D236" s="101" t="s">
-        <v>21</v>
-      </c>
-      <c r="E236" s="101" t="s">
-        <v>68</v>
-      </c>
-      <c r="F236" s="101" t="s">
-        <v>26</v>
-      </c>
-      <c r="G236" s="100">
-        <v>14</v>
-      </c>
-      <c r="H236" s="100">
-        <v>10</v>
-      </c>
-      <c r="I236" s="100">
-        <v>3</v>
-      </c>
-      <c r="J236" s="100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="237" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B237" s="100" t="s">
-        <v>229</v>
-      </c>
-      <c r="C237" s="100" t="s">
-        <v>238</v>
-      </c>
-      <c r="D237" s="101" t="s">
-        <v>21</v>
-      </c>
-      <c r="E237" s="101" t="s">
-        <v>68</v>
-      </c>
-      <c r="F237" s="101" t="s">
-        <v>26</v>
-      </c>
-      <c r="G237" s="100">
-        <v>7</v>
-      </c>
-      <c r="H237" s="100">
-        <v>7</v>
-      </c>
-      <c r="I237" s="100">
-        <v>5</v>
-      </c>
-      <c r="J237" s="100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:10" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A238" s="81">
-        <v>76</v>
-      </c>
-      <c r="B238" s="100" t="s">
-        <v>231</v>
-      </c>
-      <c r="C238" s="100" t="s">
-        <v>238</v>
-      </c>
-      <c r="D238" s="101" t="s">
-        <v>28</v>
-      </c>
-      <c r="E238" s="101" t="s">
-        <v>68</v>
-      </c>
-      <c r="F238" s="101" t="s">
-        <v>26</v>
-      </c>
-      <c r="G238" s="100">
-        <v>5</v>
-      </c>
-      <c r="H238" s="100">
-        <v>5</v>
-      </c>
-      <c r="I238" s="100">
-        <v>2</v>
-      </c>
-      <c r="J238" s="100">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C200:C205">
@@ -19007,7 +18730,7 @@
         <v>73</v>
       </c>
       <c r="B1" s="103" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C1" s="104" t="s">
         <v>222</v>
@@ -19078,7 +18801,7 @@
         <v>73</v>
       </c>
       <c r="B2" s="113" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C2" s="114" t="s">
         <v>222</v>
@@ -19149,7 +18872,7 @@
         <v>73</v>
       </c>
       <c r="B3" s="116" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C3" s="104" t="s">
         <v>222</v>
@@ -19220,7 +18943,7 @@
         <v>73</v>
       </c>
       <c r="B4" s="113" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C4" s="114" t="s">
         <v>222</v>
@@ -19291,7 +19014,7 @@
         <v>73</v>
       </c>
       <c r="B5" s="116" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C5" s="104" t="s">
         <v>222</v>
@@ -19362,7 +19085,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C6" s="114" t="s">
         <v>222</v>
@@ -19433,7 +19156,7 @@
         <v>76</v>
       </c>
       <c r="B7" s="116" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C7" s="104" t="s">
         <v>222</v>
@@ -19504,7 +19227,7 @@
         <v>76</v>
       </c>
       <c r="B8" s="113" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C8" s="114" t="s">
         <v>222</v>
@@ -19575,7 +19298,7 @@
         <v>73</v>
       </c>
       <c r="B9" s="126" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C9" s="127" t="s">
         <v>233</v>
@@ -19667,14 +19390,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19913,21 +19634,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0ECD7C-9783-4AF2-B19D-668092346D66}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d777fa6b-bca0-4864-8d50-ac77b155e846"/>
-    <ds:schemaRef ds:uri="c0eeac73-9918-465e-bdd8-785547fbc2d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19952,9 +19672,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0ECD7C-9783-4AF2-B19D-668092346D66}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d777fa6b-bca0-4864-8d50-ac77b155e846"/>
+    <ds:schemaRef ds:uri="c0eeac73-9918-465e-bdd8-785547fbc2d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
add age pen stats
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cbussuper.sharepoint.com/sites/MarketingTechTeam/Shared Documents/Reporting/FY26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EB6D736-BD17-4648-84E3-F58F9685CA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E016FD0D-321E-4B4B-B08B-60C3CA687854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -294,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="297">
   <si>
     <t>img-id</t>
   </si>
@@ -1159,6 +1159,18 @@
   </si>
   <si>
     <t>https://litmus.com/folders/324180/emails/20279341/analytics</t>
+  </si>
+  <si>
+    <t>Age Pension - 68 Years (Filterted stats from insight team)</t>
+  </si>
+  <si>
+    <t>Age Pension - 67 Years  (Filterted stats from insight team)</t>
+  </si>
+  <si>
+    <t>Age Pension - 66 Years (Filterted stats from insight team)</t>
+  </si>
+  <si>
+    <t>Age Pension - 57 Years  (Filterted stats from insight team)</t>
   </si>
   <si>
     <t>Averages %</t>
@@ -1560,7 +1572,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" indent="1"/>
@@ -1895,6 +1907,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2636,8 +2660,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="A1:T275" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21">
-  <autoFilter ref="A1:T275" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="A1:T279" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21">
+  <autoFilter ref="A1:T279" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T160">
     <sortCondition ref="C1:C160"/>
   </sortState>
@@ -2999,11 +3023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23CF1A7-A843-E143-B142-84B9EDCB7AA1}">
-  <dimension ref="A1:T275"/>
+  <dimension ref="A1:T279"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G264" sqref="G264"/>
+      <pane ySplit="1" topLeftCell="K272" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q276" sqref="Q276:T278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="32.1" customHeight="1"/>
@@ -21938,6 +21962,258 @@
       <c r="T275" s="117" t="s">
         <v>287</v>
       </c>
+    </row>
+    <row r="276" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A276" s="81">
+        <v>23</v>
+      </c>
+      <c r="B276" s="108" t="s">
+        <v>288</v>
+      </c>
+      <c r="C276" s="70">
+        <v>45992</v>
+      </c>
+      <c r="D276" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E276" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F276" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G276" s="9">
+        <v>193</v>
+      </c>
+      <c r="H276" s="25">
+        <v>120</v>
+      </c>
+      <c r="I276" s="29">
+        <v>16</v>
+      </c>
+      <c r="J276" s="16">
+        <v>0</v>
+      </c>
+      <c r="K276" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L276" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>62.176165803108809</v>
+      </c>
+      <c r="M276" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>8.2901554404145088</v>
+      </c>
+      <c r="N276" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="O276" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>38.154044403876611</v>
+      </c>
+      <c r="P276" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🟡</v>
+      </c>
+      <c r="Q276" s="124"/>
+      <c r="R276" s="124"/>
+      <c r="S276" s="124"/>
+      <c r="T276" s="127"/>
+    </row>
+    <row r="277" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A277" s="81">
+        <v>22</v>
+      </c>
+      <c r="B277" s="108" t="s">
+        <v>289</v>
+      </c>
+      <c r="C277" s="70">
+        <v>45992</v>
+      </c>
+      <c r="D277" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E277" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F277" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G277" s="9">
+        <v>226</v>
+      </c>
+      <c r="H277" s="25">
+        <v>161</v>
+      </c>
+      <c r="I277" s="29">
+        <v>59</v>
+      </c>
+      <c r="J277" s="11">
+        <v>0</v>
+      </c>
+      <c r="K277" s="36">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L277" s="6">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>71.238938053097343</v>
+      </c>
+      <c r="M277" s="31">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>26.10619469026549</v>
+      </c>
+      <c r="N277" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>36.645962732919259</v>
+      </c>
+      <c r="O277" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>61.379121309421251</v>
+      </c>
+      <c r="P277" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🟢</v>
+      </c>
+      <c r="Q277" s="124"/>
+      <c r="R277" s="124"/>
+      <c r="S277" s="124"/>
+      <c r="T277" s="127"/>
+    </row>
+    <row r="278" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A278" s="81">
+        <v>21</v>
+      </c>
+      <c r="B278" s="108" t="s">
+        <v>290</v>
+      </c>
+      <c r="C278" s="70">
+        <v>45992</v>
+      </c>
+      <c r="D278" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E278" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F278" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G278" s="9">
+        <v>214</v>
+      </c>
+      <c r="H278" s="25">
+        <v>123</v>
+      </c>
+      <c r="I278" s="29">
+        <v>22</v>
+      </c>
+      <c r="J278" s="16">
+        <v>0</v>
+      </c>
+      <c r="K278" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L278" s="44">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>57.476635514018696</v>
+      </c>
+      <c r="M278" s="45">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>10.2803738317757</v>
+      </c>
+      <c r="N278" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>17.886178861788618</v>
+      </c>
+      <c r="O278" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>37.361341601886629</v>
+      </c>
+      <c r="P278" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🟡</v>
+      </c>
+      <c r="Q278" s="124"/>
+      <c r="R278" s="124"/>
+      <c r="S278" s="124"/>
+      <c r="T278" s="127"/>
+    </row>
+    <row r="279" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A279" s="82">
+        <v>20</v>
+      </c>
+      <c r="B279" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="C279" s="70">
+        <v>45992</v>
+      </c>
+      <c r="D279" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="E279" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F279" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G279" s="13">
+        <v>428</v>
+      </c>
+      <c r="H279" s="24">
+        <v>210</v>
+      </c>
+      <c r="I279" s="28">
+        <v>17</v>
+      </c>
+      <c r="J279" s="16">
+        <v>2</v>
+      </c>
+      <c r="K279" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0.46728971962616817</v>
+      </c>
+      <c r="L279" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>49.065420560747661</v>
+      </c>
+      <c r="M279" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>3.9719626168224296</v>
+      </c>
+      <c r="N279" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>8.0952380952380949</v>
+      </c>
+      <c r="O279" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>26.637424665909684</v>
+      </c>
+      <c r="P279" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🔴</v>
+      </c>
+      <c r="Q279" s="125"/>
+      <c r="R279" s="125"/>
+      <c r="S279" s="125"/>
+      <c r="T279" s="126"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C197:C202">
@@ -22335,11 +22611,15 @@
     <hyperlink ref="T273" r:id="rId354" xr:uid="{64F605DE-53A2-4520-9ECB-700F494E4B56}"/>
     <hyperlink ref="T274" r:id="rId355" xr:uid="{F6F05B44-6AA2-4B51-A325-43FB7485F862}"/>
     <hyperlink ref="T275" r:id="rId356" xr:uid="{6FA4FBEE-9AD9-4F61-8D10-C7C9A74A177F}"/>
+    <hyperlink ref="B276" r:id="rId357" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{90EA5B2E-0B7B-4C4F-837D-0A6B5A5040E0}"/>
+    <hyperlink ref="B277" r:id="rId358" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{80F0ADC7-54B7-4261-8899-88744AEFCE9F}"/>
+    <hyperlink ref="B278" r:id="rId359" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{38563F74-846E-4FAD-99DB-EB52E1F2AE65}"/>
+    <hyperlink ref="B279" r:id="rId360" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{8ADD44E8-6354-42E1-BB12-830FDE27E91D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId357"/>
+  <legacyDrawing r:id="rId361"/>
   <tableParts count="1">
-    <tablePart r:id="rId358"/>
+    <tablePart r:id="rId362"/>
   </tableParts>
 </worksheet>
 </file>
@@ -22360,44 +22640,44 @@
   <sheetData>
     <row r="1" spans="1:2" s="120" customFormat="1">
       <c r="A1" s="121" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="B1" s="119"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="122" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="B2" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!L:L))</f>
-        <v>64.768442863437429</v>
+        <v>64.699678073787155</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="122" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="B3" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!M:M))</f>
-        <v>6.4166952030591622</v>
+        <v>6.4993639288398866</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="122" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="B4" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!N:N))</f>
-        <v>9.8200283852527317</v>
+        <v>9.9519729877069345</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="122" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B5" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!K:K))</f>
-        <v>0.15054122509451209</v>
+        <v>0.15005606257382187</v>
       </c>
     </row>
   </sheetData>
@@ -22406,6 +22686,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005CAB1339F159CD428AD0F5BA99C368F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3c12e32d35f281fc2cfbff59ce227b1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0eeac73-9918-465e-bdd8-785547fbc2d9" xmlns:ns3="d777fa6b-bca0-4864-8d50-ac77b155e846" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8cccd8974b01cfe5577657fdcd6042cb" ns2:_="" ns3:_="">
     <xsd:import namespace="c0eeac73-9918-465e-bdd8-785547fbc2d9"/>
@@ -22640,17 +22931,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -22661,11 +22941,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EBF9AAC-F6EE-4F9D-A850-BD5FE7C93CA6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EBF9AAC-F6EE-4F9D-A850-BD5FE7C93CA6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
update PYS MS 9m
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cbussuper.sharepoint.com/sites/MarketingTechTeam/Shared Documents/Reporting/FY26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E016FD0D-321E-4B4B-B08B-60C3CA687854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CCC12F6-761E-4E67-A1B9-E0A2F4641D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -294,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="298">
   <si>
     <t>img-id</t>
   </si>
@@ -1143,6 +1143,21 @@
     <t xml:space="preserve">Data Capture- Accum </t>
   </si>
   <si>
+    <t xml:space="preserve">PYS 9 Months (22-Dec-End) </t>
+  </si>
+  <si>
+    <t>Age Pension - 68 Years (Filterted stats from insight team)</t>
+  </si>
+  <si>
+    <t>Age Pension - 67 Years  (Filterted stats from insight team)</t>
+  </si>
+  <si>
+    <t>Age Pension - 66 Years (Filterted stats from insight team)</t>
+  </si>
+  <si>
+    <t>Age Pension - 57 Years  (Filterted stats from insight team)</t>
+  </si>
+  <si>
     <t xml:space="preserve">CBUS - Podcast Launch [Super Shift] </t>
   </si>
   <si>
@@ -1159,18 +1174,6 @@
   </si>
   <si>
     <t>https://litmus.com/folders/324180/emails/20279341/analytics</t>
-  </si>
-  <si>
-    <t>Age Pension - 68 Years (Filterted stats from insight team)</t>
-  </si>
-  <si>
-    <t>Age Pension - 67 Years  (Filterted stats from insight team)</t>
-  </si>
-  <si>
-    <t>Age Pension - 66 Years (Filterted stats from insight team)</t>
-  </si>
-  <si>
-    <t>Age Pension - 57 Years  (Filterted stats from insight team)</t>
   </si>
   <si>
     <t>Averages %</t>
@@ -1909,16 +1912,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2660,8 +2663,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="A1:T279" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21">
-  <autoFilter ref="A1:T279" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}" name="Table1" displayName="Table1" ref="A1:T281" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21">
+  <autoFilter ref="A1:T281" xr:uid="{50DD768E-A427-4502-A92D-DAA15A17B5EF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T160">
     <sortCondition ref="C1:C160"/>
   </sortState>
@@ -3023,11 +3026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23CF1A7-A843-E143-B142-84B9EDCB7AA1}">
-  <dimension ref="A1:T279"/>
+  <dimension ref="A1:T281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="K272" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q276" sqref="Q276:T278"/>
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A275" sqref="A275:XFD275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="32.1" customHeight="1"/>
@@ -21701,7 +21704,7 @@
         <v>23</v>
       </c>
       <c r="G272" s="13">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H272" s="24">
         <v>57</v>
@@ -21718,11 +21721,11 @@
       </c>
       <c r="L272" s="21">
         <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>61.29032258064516</v>
+        <v>61.95652173913043</v>
       </c>
       <c r="M272" s="37">
         <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>2.1505376344086025</v>
+        <v>2.1739130434782608</v>
       </c>
       <c r="N272" s="37">
         <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
@@ -21733,7 +21736,7 @@
  + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
  * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
  - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>32.402589894785521</v>
+        <v>32.762287334593573</v>
       </c>
       <c r="P272" s="37" t="str">
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
@@ -21751,469 +21754,603 @@
       <c r="T272" s="98"/>
     </row>
     <row r="273" spans="1:20" ht="32.1" customHeight="1">
-      <c r="A273" s="82">
-        <v>94</v>
-      </c>
-      <c r="B273" s="86" t="s">
+      <c r="A273" s="81">
+        <v>79</v>
+      </c>
+      <c r="B273" s="84" t="s">
         <v>282</v>
       </c>
       <c r="C273" s="70">
-        <v>46000</v>
-      </c>
-      <c r="D273" s="15" t="s">
+        <v>45992</v>
+      </c>
+      <c r="D273" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="E273" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F273" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G273" s="13">
-        <v>161516</v>
-      </c>
-      <c r="H273" s="24">
-        <v>76045</v>
-      </c>
-      <c r="I273" s="28">
-        <v>3030</v>
-      </c>
-      <c r="J273" s="16">
-        <v>132</v>
+      <c r="E273" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F273" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G273" s="9">
+        <v>1495</v>
+      </c>
+      <c r="H273" s="25">
+        <v>1008</v>
+      </c>
+      <c r="I273" s="29">
+        <v>147</v>
+      </c>
+      <c r="J273" s="60">
+        <v>3</v>
       </c>
       <c r="K273" s="35">
         <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>8.172564947125982E-2</v>
+        <v>0.20066889632107021</v>
       </c>
       <c r="L273" s="21">
         <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>47.082022833651152</v>
+        <v>67.424749163879596</v>
       </c>
       <c r="M273" s="37">
         <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>1.8759751355902818</v>
+        <v>9.8327759197324429</v>
       </c>
       <c r="N273" s="37">
         <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>3.984482871983694</v>
+        <v>14.583333333333334</v>
       </c>
       <c r="O273" s="37">
         <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
  + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
  * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
  - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>24.774767620071078</v>
+        <v>42.02570441046521</v>
       </c>
       <c r="P273" s="37" t="str">
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
-        <v>🔴</v>
-      </c>
-      <c r="Q273" s="14">
-        <v>73.2</v>
-      </c>
-      <c r="R273" s="16">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="S273" s="16">
-        <v>10.7</v>
-      </c>
-      <c r="T273" s="99" t="s">
+        <v>🟢</v>
+      </c>
+      <c r="Q273" s="60"/>
+      <c r="R273" s="60"/>
+      <c r="S273" s="60"/>
+      <c r="T273" s="87"/>
+    </row>
+    <row r="274" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A274" s="81">
+        <v>45</v>
+      </c>
+      <c r="B274" s="84" t="s">
+        <v>282</v>
+      </c>
+      <c r="C274" s="70">
+        <v>45992</v>
+      </c>
+      <c r="D274" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E274" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F274" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G274" s="9">
+        <v>60</v>
+      </c>
+      <c r="H274" s="25">
+        <v>37</v>
+      </c>
+      <c r="I274" s="29">
+        <v>3</v>
+      </c>
+      <c r="J274" s="60">
+        <v>0</v>
+      </c>
+      <c r="K274" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L274" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>61.666666666666671</v>
+      </c>
+      <c r="M274" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>5</v>
+      </c>
+      <c r="N274" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>8.1081081081081088</v>
+      </c>
+      <c r="O274" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>35.000000000000007</v>
+      </c>
+      <c r="P274" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🟡</v>
+      </c>
+      <c r="Q274" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="R274" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="S274" s="60" t="s">
+        <v>185</v>
+      </c>
+      <c r="T274" s="87" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="275" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A275" s="81">
+        <v>23</v>
+      </c>
+      <c r="B275" s="108" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="274" spans="1:20" ht="32.1" customHeight="1">
-      <c r="A274" s="82">
-        <v>95</v>
-      </c>
-      <c r="B274" s="104" t="s">
-        <v>284</v>
-      </c>
-      <c r="C274" s="70">
-        <v>46009</v>
-      </c>
-      <c r="D274" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E274" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F274" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G274" s="13">
-        <v>169</v>
-      </c>
-      <c r="H274" s="24">
-        <v>123</v>
-      </c>
-      <c r="I274" s="28">
-        <v>5</v>
-      </c>
-      <c r="J274" s="16">
-        <v>0</v>
-      </c>
-      <c r="K274" s="35">
-        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>0</v>
-      </c>
-      <c r="L274" s="21">
-        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>72.781065088757401</v>
-      </c>
-      <c r="M274" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>2.9585798816568047</v>
-      </c>
-      <c r="N274" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>4.0650406504065035</v>
-      </c>
-      <c r="O274" s="37">
-        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
- + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
- * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
- - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>38.990231434473579</v>
-      </c>
-      <c r="P274" s="37" t="str">
+      <c r="C275" s="70">
+        <v>45992</v>
+      </c>
+      <c r="D275" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E275" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F275" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G275" s="9">
+        <v>193</v>
+      </c>
+      <c r="H275" s="25">
+        <v>120</v>
+      </c>
+      <c r="I275" s="29">
+        <v>16</v>
+      </c>
+      <c r="J275" s="16">
+        <v>0</v>
+      </c>
+      <c r="K275" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L275" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>62.176165803108809</v>
+      </c>
+      <c r="M275" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>8.2901554404145088</v>
+      </c>
+      <c r="N275" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="O275" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>38.154044403876611</v>
+      </c>
+      <c r="P275" s="37" t="str">
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
         <v>🟡</v>
       </c>
-      <c r="Q274" s="14">
-        <v>40</v>
-      </c>
-      <c r="R274" s="16">
-        <v>26.7</v>
-      </c>
-      <c r="S274" s="16">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="T274" s="117" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="275" spans="1:20" ht="32.1" customHeight="1">
-      <c r="A275" s="82">
-        <v>95</v>
-      </c>
-      <c r="B275" s="104" t="s">
-        <v>286</v>
-      </c>
-      <c r="C275" s="70">
-        <v>46009</v>
-      </c>
-      <c r="D275" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E275" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F275" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G275" s="13">
-        <v>2754</v>
-      </c>
-      <c r="H275" s="24">
-        <v>1665</v>
-      </c>
-      <c r="I275" s="28">
-        <v>181</v>
-      </c>
-      <c r="J275" s="16">
-        <v>1</v>
-      </c>
-      <c r="K275" s="35">
-        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>3.6310820624546117E-2</v>
-      </c>
-      <c r="L275" s="21">
-        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>60.457516339869279</v>
-      </c>
-      <c r="M275" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>6.572258533042846</v>
-      </c>
-      <c r="N275" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>10.870870870870871</v>
-      </c>
-      <c r="O275" s="37">
-        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
- + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
- * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
- - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>35.644950844589161</v>
-      </c>
-      <c r="P275" s="37" t="str">
-        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
-        <v>🟡</v>
-      </c>
-      <c r="Q275" s="14">
-        <v>77.2</v>
-      </c>
-      <c r="R275" s="16">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="S275" s="16">
-        <v>6.4</v>
-      </c>
-      <c r="T275" s="117" t="s">
-        <v>287</v>
-      </c>
+      <c r="Q275" s="60"/>
+      <c r="R275" s="60"/>
+      <c r="S275" s="60"/>
+      <c r="T275" s="124"/>
     </row>
     <row r="276" spans="1:20" ht="32.1" customHeight="1">
       <c r="A276" s="81">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B276" s="108" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C276" s="70">
         <v>45992</v>
       </c>
-      <c r="D276" s="46" t="s">
+      <c r="D276" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="E276" s="46" t="s">
+      <c r="E276" s="48" t="s">
         <v>22</v>
       </c>
       <c r="F276" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G276" s="9">
-        <v>193</v>
+        <v>226</v>
       </c>
       <c r="H276" s="25">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="I276" s="29">
-        <v>16</v>
-      </c>
-      <c r="J276" s="16">
-        <v>0</v>
-      </c>
-      <c r="K276" s="35">
-        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>0</v>
-      </c>
-      <c r="L276" s="21">
-        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>62.176165803108809</v>
-      </c>
-      <c r="M276" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>8.2901554404145088</v>
+        <v>59</v>
+      </c>
+      <c r="J276" s="11">
+        <v>0</v>
+      </c>
+      <c r="K276" s="36">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L276" s="6">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>71.238938053097343</v>
+      </c>
+      <c r="M276" s="31">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>26.10619469026549</v>
       </c>
       <c r="N276" s="37">
         <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>13.333333333333334</v>
+        <v>36.645962732919259</v>
       </c>
       <c r="O276" s="37">
         <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
  + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
  * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
  - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>38.154044403876611</v>
+        <v>61.379121309421251</v>
       </c>
       <c r="P276" s="37" t="str">
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
-        <v>🟡</v>
-      </c>
-      <c r="Q276" s="124"/>
-      <c r="R276" s="124"/>
-      <c r="S276" s="124"/>
-      <c r="T276" s="127"/>
+        <v>🟢</v>
+      </c>
+      <c r="Q276" s="60"/>
+      <c r="R276" s="60"/>
+      <c r="S276" s="60"/>
+      <c r="T276" s="124"/>
     </row>
     <row r="277" spans="1:20" ht="32.1" customHeight="1">
       <c r="A277" s="81">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B277" s="108" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C277" s="70">
         <v>45992</v>
       </c>
-      <c r="D277" s="48" t="s">
+      <c r="D277" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="E277" s="48" t="s">
+      <c r="E277" s="46" t="s">
         <v>22</v>
       </c>
       <c r="F277" s="20" t="s">
         <v>23</v>
       </c>
       <c r="G277" s="9">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="H277" s="25">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="I277" s="29">
-        <v>59</v>
-      </c>
-      <c r="J277" s="11">
-        <v>0</v>
-      </c>
-      <c r="K277" s="36">
-        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>0</v>
-      </c>
-      <c r="L277" s="6">
-        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>71.238938053097343</v>
-      </c>
-      <c r="M277" s="31">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>26.10619469026549</v>
+        <v>22</v>
+      </c>
+      <c r="J277" s="16">
+        <v>0</v>
+      </c>
+      <c r="K277" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L277" s="44">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>57.476635514018696</v>
+      </c>
+      <c r="M277" s="45">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>10.2803738317757</v>
       </c>
       <c r="N277" s="37">
         <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>36.645962732919259</v>
+        <v>17.886178861788618</v>
       </c>
       <c r="O277" s="37">
         <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
  + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
  * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
  - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>61.379121309421251</v>
+        <v>37.361341601886629</v>
       </c>
       <c r="P277" s="37" t="str">
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
-        <v>🟢</v>
-      </c>
-      <c r="Q277" s="124"/>
-      <c r="R277" s="124"/>
-      <c r="S277" s="124"/>
-      <c r="T277" s="127"/>
+        <v>🟡</v>
+      </c>
+      <c r="Q277" s="60"/>
+      <c r="R277" s="60"/>
+      <c r="S277" s="60"/>
+      <c r="T277" s="124"/>
     </row>
     <row r="278" spans="1:20" ht="32.1" customHeight="1">
-      <c r="A278" s="81">
-        <v>21</v>
-      </c>
-      <c r="B278" s="108" t="s">
-        <v>290</v>
+      <c r="A278" s="82">
+        <v>20</v>
+      </c>
+      <c r="B278" s="111" t="s">
+        <v>286</v>
       </c>
       <c r="C278" s="70">
         <v>45992</v>
       </c>
-      <c r="D278" s="46" t="s">
+      <c r="D278" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="E278" s="46" t="s">
+      <c r="E278" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="F278" s="20" t="s">
+      <c r="F278" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G278" s="9">
-        <v>214</v>
-      </c>
-      <c r="H278" s="25">
+      <c r="G278" s="13">
+        <v>428</v>
+      </c>
+      <c r="H278" s="24">
+        <v>210</v>
+      </c>
+      <c r="I278" s="28">
+        <v>17</v>
+      </c>
+      <c r="J278" s="16">
+        <v>2</v>
+      </c>
+      <c r="K278" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0.46728971962616817</v>
+      </c>
+      <c r="L278" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>49.065420560747661</v>
+      </c>
+      <c r="M278" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>3.9719626168224296</v>
+      </c>
+      <c r="N278" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>8.0952380952380949</v>
+      </c>
+      <c r="O278" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>26.637424665909684</v>
+      </c>
+      <c r="P278" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🔴</v>
+      </c>
+      <c r="Q278" s="60"/>
+      <c r="R278" s="60"/>
+      <c r="S278" s="60"/>
+      <c r="T278" s="87"/>
+    </row>
+    <row r="279" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A279" s="81">
+        <v>94</v>
+      </c>
+      <c r="B279" s="106" t="s">
+        <v>287</v>
+      </c>
+      <c r="C279" s="69">
+        <v>46000</v>
+      </c>
+      <c r="D279" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="E279" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F279" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G279" s="9">
+        <v>161516</v>
+      </c>
+      <c r="H279" s="25">
+        <v>76045</v>
+      </c>
+      <c r="I279" s="29">
+        <v>3030</v>
+      </c>
+      <c r="J279" s="16">
+        <v>132</v>
+      </c>
+      <c r="K279" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>8.172564947125982E-2</v>
+      </c>
+      <c r="L279" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>47.082022833651152</v>
+      </c>
+      <c r="M279" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>1.8759751355902818</v>
+      </c>
+      <c r="N279" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>3.984482871983694</v>
+      </c>
+      <c r="O279" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>24.774767620071078</v>
+      </c>
+      <c r="P279" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🔴</v>
+      </c>
+      <c r="Q279" s="125">
+        <v>73.2</v>
+      </c>
+      <c r="R279" s="126">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="S279" s="126">
+        <v>10.7</v>
+      </c>
+      <c r="T279" s="127" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="280" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A280" s="81">
+        <v>95</v>
+      </c>
+      <c r="B280" s="106" t="s">
+        <v>289</v>
+      </c>
+      <c r="C280" s="69">
+        <v>46009</v>
+      </c>
+      <c r="D280" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E280" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F280" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G280" s="9">
+        <v>169</v>
+      </c>
+      <c r="H280" s="25">
         <v>123</v>
       </c>
-      <c r="I278" s="29">
-        <v>22</v>
-      </c>
-      <c r="J278" s="16">
-        <v>0</v>
-      </c>
-      <c r="K278" s="35">
-        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>0</v>
-      </c>
-      <c r="L278" s="44">
-        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>57.476635514018696</v>
-      </c>
-      <c r="M278" s="45">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>10.2803738317757</v>
-      </c>
-      <c r="N278" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>17.886178861788618</v>
-      </c>
-      <c r="O278" s="37">
-        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
- + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
- * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
- - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>37.361341601886629</v>
-      </c>
-      <c r="P278" s="37" t="str">
+      <c r="I280" s="29">
+        <v>5</v>
+      </c>
+      <c r="J280" s="16">
+        <v>0</v>
+      </c>
+      <c r="K280" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>0</v>
+      </c>
+      <c r="L280" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>72.781065088757401</v>
+      </c>
+      <c r="M280" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>2.9585798816568047</v>
+      </c>
+      <c r="N280" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>4.0650406504065035</v>
+      </c>
+      <c r="O280" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>38.990231434473579</v>
+      </c>
+      <c r="P280" s="37" t="str">
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
         <v>🟡</v>
       </c>
-      <c r="Q278" s="124"/>
-      <c r="R278" s="124"/>
-      <c r="S278" s="124"/>
-      <c r="T278" s="127"/>
-    </row>
-    <row r="279" spans="1:20" ht="32.1" customHeight="1">
-      <c r="A279" s="82">
-        <v>20</v>
-      </c>
-      <c r="B279" s="111" t="s">
+      <c r="Q280" s="125">
+        <v>40</v>
+      </c>
+      <c r="R280" s="126">
+        <v>26.7</v>
+      </c>
+      <c r="S280" s="126">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="T280" s="127" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="281" spans="1:20" ht="32.1" customHeight="1">
+      <c r="A281" s="82">
+        <v>95</v>
+      </c>
+      <c r="B281" s="104" t="s">
         <v>291</v>
       </c>
-      <c r="C279" s="70">
-        <v>45992</v>
-      </c>
-      <c r="D279" s="47" t="s">
+      <c r="C281" s="70">
+        <v>46009</v>
+      </c>
+      <c r="D281" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E279" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="F279" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G279" s="13">
-        <v>428</v>
-      </c>
-      <c r="H279" s="24">
-        <v>210</v>
-      </c>
-      <c r="I279" s="28">
-        <v>17</v>
-      </c>
-      <c r="J279" s="16">
-        <v>2</v>
-      </c>
-      <c r="K279" s="35">
-        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
-        <v>0.46728971962616817</v>
-      </c>
-      <c r="L279" s="21">
-        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>49.065420560747661</v>
-      </c>
-      <c r="M279" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
-        <v>3.9719626168224296</v>
-      </c>
-      <c r="N279" s="37">
-        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
-        <v>8.0952380952380949</v>
-      </c>
-      <c r="O279" s="37">
-        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
- + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
- * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
- - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
-        <v>26.637424665909684</v>
-      </c>
-      <c r="P279" s="37" t="str">
-        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
-        <v>🔴</v>
-      </c>
-      <c r="Q279" s="125"/>
-      <c r="R279" s="125"/>
-      <c r="S279" s="125"/>
-      <c r="T279" s="126"/>
+      <c r="E281" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="F281" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G281" s="13">
+        <v>2754</v>
+      </c>
+      <c r="H281" s="24">
+        <v>1665</v>
+      </c>
+      <c r="I281" s="28">
+        <v>181</v>
+      </c>
+      <c r="J281" s="16">
+        <v>1</v>
+      </c>
+      <c r="K281" s="35">
+        <f>(Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]])*100</f>
+        <v>3.6310820624546117E-2</v>
+      </c>
+      <c r="L281" s="21">
+        <f>Table1[[#This Row],[unique-opens]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>60.457516339869279</v>
+      </c>
+      <c r="M281" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-sends]] * 100</f>
+        <v>6.572258533042846</v>
+      </c>
+      <c r="N281" s="37">
+        <f>Table1[[#This Row],[unique-clicks]] / Table1[[#This Row],[unique-opens]] * 100</f>
+        <v>10.870870870870871</v>
+      </c>
+      <c r="O281" s="37">
+        <f>(MIN(Table1[[#This Row],[unique-opens]]/Table1[[#This Row],[unique-sends]],1)*50
+ + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1)*50)
+ * (1 + MIN(Table1[[#This Row],[unique-clicks]]/Table1[[#This Row],[unique-sends]],1))
+ - ((Table1[[#This Row],[unsub]]/Table1[[#This Row],[unique-sends]]*100)*2)</f>
+        <v>35.644950844589161</v>
+      </c>
+      <c r="P281" s="37" t="str">
+        <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
+        <v>🟡</v>
+      </c>
+      <c r="Q281" s="125">
+        <v>77.2</v>
+      </c>
+      <c r="R281" s="126">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="S281" s="126">
+        <v>6.4</v>
+      </c>
+      <c r="T281" s="127" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C197:C202">
@@ -22255,371 +22392,349 @@
     <cfRule type="duplicateValues" dxfId="24" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/541e1d3f-d064-4e8c-ad26-a2f26946d5ec" xr:uid="{A0444A8C-B658-434F-912C-6E4903003899}"/>
-    <hyperlink ref="B32" r:id="rId2" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{7F7AB8F8-DEAF-3449-99E1-B7BA87B8D6EF}"/>
-    <hyperlink ref="B33" r:id="rId3" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{B63C576D-7994-6D43-BAC0-C9CB36419E3D}"/>
-    <hyperlink ref="B28" r:id="rId4" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{55F1AE99-10CB-7148-815A-490ABAE8C7E5}"/>
-    <hyperlink ref="B29" r:id="rId5" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{E086D344-6939-0546-BD48-E1DE212F93A3}"/>
-    <hyperlink ref="B30" r:id="rId6" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{BA7A759B-B2FB-C64C-AACF-2D62F08DC76A}"/>
-    <hyperlink ref="B31" r:id="rId7" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{4D168887-CA13-A245-A790-692A0821F674}"/>
-    <hyperlink ref="B34" r:id="rId8" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{A74DA7AF-FF8B-CD43-A7F7-7E57FBD2A7BA}"/>
-    <hyperlink ref="B35" r:id="rId9" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{0DCFFBD3-AB88-B84D-96F9-F86FD4E67D64}"/>
-    <hyperlink ref="B37" r:id="rId10" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{6DF15277-6029-7343-8803-C69575ED3570}"/>
-    <hyperlink ref="B36" r:id="rId11" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="EOFY Performance" xr:uid="{4F2D85B6-4267-0641-8B81-5023B9593C70}"/>
-    <hyperlink ref="B38" r:id="rId12" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="EOFY Performance" xr:uid="{B316FBC2-9FEE-B340-A267-E6ECABFCA375}"/>
-    <hyperlink ref="B39" r:id="rId13" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="EOFY Performance" xr:uid="{ED60402C-1452-B241-8941-D6448A79EB4B}"/>
-    <hyperlink ref="B40" r:id="rId14" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{2DDC3489-8245-B045-B27C-0C53BE66B1D3}"/>
-    <hyperlink ref="B41" r:id="rId15" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{CC18B321-7B40-B14C-B0BA-0B394F37FB1B}"/>
-    <hyperlink ref="B42" r:id="rId16" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="CBUS - Corporate insurance SEN (AME) Cbus" xr:uid="{C540744B-5256-B74D-917A-E9C3183B0ED0}"/>
-    <hyperlink ref="B43" r:id="rId17" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{D2AD9D56-ED8D-A74B-BF75-E0A47B438E34}"/>
-    <hyperlink ref="B44" r:id="rId18" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{E0417873-39DF-B845-B923-0200FA9CA2F7}"/>
-    <hyperlink ref="B49" r:id="rId19" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{D74E4B1C-FE5C-C542-800C-ECA69E65CCF0}"/>
-    <hyperlink ref="B50" r:id="rId20" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{9E4CF538-4AC2-1849-8C5A-4AB7B64B6F63}"/>
-    <hyperlink ref="B45" r:id="rId21" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{B25CC288-D429-7342-8850-3247BA70AFCE}"/>
-    <hyperlink ref="B46" r:id="rId22" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{53BC90F5-EC80-0D48-BDE3-6B226F229779}"/>
-    <hyperlink ref="B47" r:id="rId23" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{9AB33328-4010-F843-B550-8D7E64EC2CD1}"/>
-    <hyperlink ref="B48" r:id="rId24" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{1CD36E2E-A888-B64A-A43F-52462AF0D631}"/>
-    <hyperlink ref="B4" r:id="rId25" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/541e1d3f-d064-4e8c-ad26-a2f26946d5ec" xr:uid="{BFA6D6B9-0F92-4A98-BC01-3F66ECBAF652}"/>
-    <hyperlink ref="T4" r:id="rId26" xr:uid="{51BBEF75-8B33-4A54-A5A5-C3E2872BA63D}"/>
-    <hyperlink ref="T3" r:id="rId27" xr:uid="{9B91B3EB-9AC1-4462-A67A-81961D7FCB79}"/>
-    <hyperlink ref="T32" r:id="rId28" xr:uid="{1077084C-D29E-4ABC-BD53-A05F91719125}"/>
-    <hyperlink ref="T33" r:id="rId29" xr:uid="{E82B6BA4-E16F-492E-BCD8-911C556EA12C}"/>
-    <hyperlink ref="T28" r:id="rId30" xr:uid="{6184ED25-1DF9-49D3-AC87-98D010A3B3E0}"/>
-    <hyperlink ref="T29" r:id="rId31" xr:uid="{23489B88-1AF7-440D-82A5-D2C99B402CE1}"/>
-    <hyperlink ref="T30" r:id="rId32" xr:uid="{29D38B7B-0EEB-4F1D-BD67-2FE0B692C886}"/>
-    <hyperlink ref="T31" r:id="rId33" xr:uid="{E529B59E-BC39-41D7-A6B8-B76C65B02964}"/>
-    <hyperlink ref="T34" r:id="rId34" xr:uid="{75D776C4-686E-4764-A0CE-7978746739AA}"/>
-    <hyperlink ref="T35" r:id="rId35" xr:uid="{18534669-D2F7-4C45-BE71-B06E441E98C4}"/>
-    <hyperlink ref="T40" r:id="rId36" xr:uid="{4456DFDD-02ED-4178-A1B2-7A56262C79A7}"/>
-    <hyperlink ref="T41" r:id="rId37" xr:uid="{85BEFFFA-77A3-49CF-94D8-7F3EBFED1A80}"/>
-    <hyperlink ref="T43" r:id="rId38" xr:uid="{9D50E18A-27F4-4E22-95C5-F200362F77FE}"/>
-    <hyperlink ref="T44" r:id="rId39" xr:uid="{49F0C4D7-6B49-48CB-9B69-3680BAAED979}"/>
-    <hyperlink ref="T49" r:id="rId40" xr:uid="{669F8622-A0EA-44FE-8AAA-EAB6EE53AEB9}"/>
-    <hyperlink ref="T50" r:id="rId41" xr:uid="{3EC869FD-833C-4252-AFF2-954077725E77}"/>
-    <hyperlink ref="B74" r:id="rId42" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2b3a8bd7-9314-4486-bed5-590aae72eef6" xr:uid="{DDE7FEFC-6B1E-4AA0-B976-36D2973B650E}"/>
-    <hyperlink ref="T74" r:id="rId43" xr:uid="{7AD33B0E-E2D3-41B8-9172-D15847D781D8}"/>
-    <hyperlink ref="B75" r:id="rId44" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/837cd468-99da-4b6c-86ed-a729c8dedaed" xr:uid="{8D543BC5-E411-41F4-AC77-9D04065517CB}"/>
-    <hyperlink ref="T75" r:id="rId45" xr:uid="{0118962C-499A-4545-8BD4-3ABE37EC8589}"/>
-    <hyperlink ref="B76" r:id="rId46" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1c60eb15-5315-4d97-bc92-f3321a8f2bb8" xr:uid="{0C3ADEAB-E937-4D0F-A344-AB2EAC09C8ED}"/>
-    <hyperlink ref="T76" r:id="rId47" xr:uid="{EA3D39DE-B821-4DE6-A6E8-54C4DB4002CB}"/>
-    <hyperlink ref="B79" r:id="rId48" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d0d232aa-3290-434d-8c3f-c589a73ea607" xr:uid="{21BFCBA6-6AD1-4DF1-BFCC-97AF53BF164E}"/>
-    <hyperlink ref="B80" r:id="rId49" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d0d232aa-3290-434d-8c3f-c589a73ea607" xr:uid="{FFD820BD-0682-4A01-886A-FC6E140DD7F6}"/>
-    <hyperlink ref="T79" r:id="rId50" xr:uid="{BDD938AD-4F2D-4D6D-A609-A2D733A83114}"/>
-    <hyperlink ref="T80" r:id="rId51" xr:uid="{54C0322F-D13C-44D8-B6EB-53DBB2BCA1C8}"/>
-    <hyperlink ref="B77" r:id="rId52" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/10c562f8-f91d-4456-8e2f-4ac211353527" xr:uid="{10A9ABF1-9B48-49EB-8857-3A95282225D7}"/>
-    <hyperlink ref="B78" r:id="rId53" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/10c562f8-f91d-4456-8e2f-4ac211353527" xr:uid="{03BE0AA5-037E-4E17-8386-29BAE9E3BEE5}"/>
-    <hyperlink ref="T77" r:id="rId54" xr:uid="{337F27CF-D0CD-4B04-A48D-36C253F1BE4F}"/>
-    <hyperlink ref="T78" r:id="rId55" xr:uid="{7FE3D493-8D5B-4496-8F77-D73CA4BD72FB}"/>
-    <hyperlink ref="B82" r:id="rId56" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2be0e003-3e51-476c-86ea-8a1f8913d899" xr:uid="{DCBBFEEB-0E31-4647-A7B8-662452421D74}"/>
-    <hyperlink ref="B83" r:id="rId57" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2be0e003-3e51-476c-86ea-8a1f8913d899" xr:uid="{F08C799E-E69A-4FAE-9577-3BE26DC55F8C}"/>
-    <hyperlink ref="T82" r:id="rId58" xr:uid="{F25A322F-4512-4FB9-896D-FC4488D151BC}"/>
-    <hyperlink ref="T83" r:id="rId59" xr:uid="{E9B325CA-DA26-471B-8892-3CD505753BC9}"/>
-    <hyperlink ref="B81" r:id="rId60" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d5aac9ae-16b6-46ce-9310-1ba0004b45ea" xr:uid="{FCD585C4-F8D5-442F-82A2-8DA88F7E9D6B}"/>
-    <hyperlink ref="T81" r:id="rId61" xr:uid="{E2C5678C-A592-4E8F-8D77-8769EA44690D}"/>
-    <hyperlink ref="B84" r:id="rId62" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cb123bc-fd8e-4868-82f1-14995d53c591" xr:uid="{930F7BAC-EDE4-4C25-8B39-8677C9CD53AD}"/>
-    <hyperlink ref="B85" r:id="rId63" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cb123bc-fd8e-4868-82f1-14995d53c591" xr:uid="{DDF5BEEE-A105-4CBA-B3EF-4B0632B51EAE}"/>
-    <hyperlink ref="T84" r:id="rId64" xr:uid="{28F02C08-2175-4786-AE8B-EF7115BB2A13}"/>
-    <hyperlink ref="T85" r:id="rId65" xr:uid="{6B6FA851-5730-41C3-9AD3-29501233C4EF}"/>
-    <hyperlink ref="B86" r:id="rId66" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/47e8e523-4417-4b5b-90e5-f72b14e59a38" display="Cbus Advocacy Research" xr:uid="{415E68FE-63DA-4727-BBF2-D5B9E5B4A68B}"/>
-    <hyperlink ref="T86" r:id="rId67" xr:uid="{2AD3FFE5-FB20-4C1E-B57F-CFE0E5B36B26}"/>
-    <hyperlink ref="B89" r:id="rId68" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/50c38354-a1aa-4221-89a9-67b1c2af5d56" xr:uid="{776AA357-15C0-415F-AD46-2E881767E760}"/>
-    <hyperlink ref="T89" r:id="rId69" xr:uid="{67874548-D942-44D2-AFBC-BB37ACD6D8B7}"/>
-    <hyperlink ref="B87" r:id="rId70" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bcdec3d6-9690-4399-8cce-1c945390b466" xr:uid="{17B72274-B78F-495D-B419-9A0D73821A7F}"/>
-    <hyperlink ref="B88" r:id="rId71" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bcdec3d6-9690-4399-8cce-1c945390b466" xr:uid="{C08F1CF4-F712-4502-B9D7-AB516367C6BC}"/>
-    <hyperlink ref="T87" r:id="rId72" xr:uid="{09AA577A-31BB-4E89-AD1C-E223A35FAD60}"/>
-    <hyperlink ref="T88" r:id="rId73" xr:uid="{720B7893-DA39-46C3-87FA-F12DA6138BED}"/>
-    <hyperlink ref="B92" r:id="rId74" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e48b4e16-bdcf-44b1-87db-8546a575ba4e" display="EOFY investment performance campaign (Microsoft HNW, SIS, Media)" xr:uid="{69BF4C00-E3BA-45B0-811B-3788561FDB24}"/>
-    <hyperlink ref="B91" r:id="rId75" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e48b4e16-bdcf-44b1-87db-8546a575ba4e" display="EOFY investment performance campaign (Microsoft HNW, SIS, Media)" xr:uid="{D7585B4B-7204-4A4E-B140-4217FD309F7E}"/>
-    <hyperlink ref="B90" r:id="rId76" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e48b4e16-bdcf-44b1-87db-8546a575ba4e" display="EOFY investment performance campaign (Microsoft HNW, SIS, Media)" xr:uid="{8256078B-EEC5-4D3C-87D3-6EDECA6A4325}"/>
-    <hyperlink ref="T91" r:id="rId77" xr:uid="{BD617822-7DD4-4BC8-8F4E-3DD549DB69D2}"/>
-    <hyperlink ref="T38" r:id="rId78" xr:uid="{43E542A7-EED9-47CD-A876-76D47F10BB49}"/>
-    <hyperlink ref="B93" r:id="rId79" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/7e56f57e-12e2-49c0-9e51-de68fe9cf789" display="#1 - SIS Acquisition - 2025 AUG" xr:uid="{E1FC8E26-35AB-43CA-8415-357E70A82AA7}"/>
-    <hyperlink ref="B95" r:id="rId80" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bca1837c-0f90-4529-9649-68676fad5162" display="#2 - SIS Acquisition - 2025 AUG" xr:uid="{83A5C014-4EB4-4268-8408-8C349E11D7B2}"/>
-    <hyperlink ref="B94" r:id="rId81" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/7e56f57e-12e2-49c0-9e51-de68fe9cf789" display="#1 - SIS Acquisition - 2025 AUG" xr:uid="{646A26CD-0D28-4643-9A18-7C11B5F2A6A6}"/>
-    <hyperlink ref="B96" r:id="rId82" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bca1837c-0f90-4529-9649-68676fad5162" display="#2 - SIS Acquisition - 2025 AUG" xr:uid="{97F55F8E-404D-4975-8457-45A84171A0DA}"/>
-    <hyperlink ref="B97" r:id="rId83" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f089ea09-6c3a-40ce-a12b-446940edf922" display="SIS Acquisition Sept 2025 - Segment 3" xr:uid="{04BC038E-0610-489D-8444-24F059E92866}"/>
-    <hyperlink ref="B99" r:id="rId84" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f089ea09-6c3a-40ce-a12b-446940edf922" display="SIS Acquisition Sept 2025 - Segment 3" xr:uid="{D5044EAD-B4FF-4896-9CE0-207234A2ACF4}"/>
-    <hyperlink ref="B98" r:id="rId85" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f089ea09-6c3a-40ce-a12b-446940edf922" display="SIS Acquisition Sept 2025 - Segment 3" xr:uid="{DE061018-F231-4EA6-B230-C6F38A03B8ED}"/>
-    <hyperlink ref="B101" r:id="rId86" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/92b3dff9-2ac0-41da-8e22-ce0ba4df098d" display="SIS Acquisition Sept 2025 - Segment 4  - Cbus" xr:uid="{90DDD61B-B442-447D-BC3F-2F85AAF8535E}"/>
-    <hyperlink ref="B100" r:id="rId87" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/92b3dff9-2ac0-41da-8e22-ce0ba4df098d" xr:uid="{405A91C1-FFD6-4110-8E98-F2CED007F2C4}"/>
-    <hyperlink ref="T93" r:id="rId88" xr:uid="{46A4C0C5-3DA2-4EDE-9262-78B2CEC51B84}"/>
-    <hyperlink ref="T94" r:id="rId89" xr:uid="{AA5FA10A-8377-4821-89EE-5352A329D287}"/>
-    <hyperlink ref="T95" r:id="rId90" xr:uid="{9AA04B41-F1EE-4344-8658-C5D6B7A1AFEA}"/>
-    <hyperlink ref="T96" r:id="rId91" xr:uid="{C2B27C02-626B-497A-93FB-13BB9D4DBBAC}"/>
-    <hyperlink ref="T99" r:id="rId92" xr:uid="{470E4EA3-F735-46B3-B163-4B6833C6BC1E}"/>
-    <hyperlink ref="T97" r:id="rId93" xr:uid="{747F63F2-3DB0-4754-92D2-72D1A8E78BE2}"/>
-    <hyperlink ref="T98" r:id="rId94" xr:uid="{5F3CB8C3-A80F-4108-86AE-76AA502ED4CE}"/>
-    <hyperlink ref="T100" r:id="rId95" xr:uid="{A4F27734-7717-4BB5-9DD8-C6FA10D03B1E}"/>
-    <hyperlink ref="T101" r:id="rId96" xr:uid="{10110FD1-EBB0-40E1-9BB7-56E1B6C67A71}"/>
-    <hyperlink ref="B130" r:id="rId97" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{7B937800-2778-4DA1-909D-7AA3E2D314AE}"/>
-    <hyperlink ref="B55" r:id="rId98" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{38AC2DFC-38D6-4B1E-8941-C0F91073E1DF}"/>
-    <hyperlink ref="B134" r:id="rId99" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{0EC00125-AD37-4C7E-87D0-E41A772F2C30}"/>
-    <hyperlink ref="B57" r:id="rId100" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{9A26CB6A-49BD-4B31-A6A4-92AF61DD4285}"/>
-    <hyperlink ref="B124" r:id="rId101" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b4838304-27ee-40d6-a2c5-fbe51637f011" display="Cbus News Sep - SIS " xr:uid="{9BB6CB4F-35CC-4CCB-A023-11C2EF4DDE69}"/>
-    <hyperlink ref="B123" r:id="rId102" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b4838304-27ee-40d6-a2c5-fbe51637f011" display="Cbus News Sep - SIS " xr:uid="{0B77C253-E7F7-42DB-81B8-1D54AEBD1DE2}"/>
-    <hyperlink ref="B127" r:id="rId103" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/738d4a66-5e39-4d8d-a98d-63f9d66dd930" display="News Sep" xr:uid="{CA7D616B-F1AE-40D0-8563-BC35B1028440}"/>
-    <hyperlink ref="T130" r:id="rId104" xr:uid="{6CD9C4AC-521A-44D2-ABED-C9ADFE5619F9}"/>
-    <hyperlink ref="T132" r:id="rId105" xr:uid="{DECC8875-831C-48D8-A401-5D8F6D6AA9A9}"/>
-    <hyperlink ref="T131" r:id="rId106" xr:uid="{9694BB1C-6051-4A63-9607-0AFC686FEDAC}"/>
-    <hyperlink ref="T134" r:id="rId107" xr:uid="{2AFB76FF-37CE-4C3B-8875-234DF8BBF9B9}"/>
-    <hyperlink ref="T136" r:id="rId108" xr:uid="{47C5D00B-E958-478C-9509-D0B2CD2EC750}"/>
-    <hyperlink ref="T135" r:id="rId109" xr:uid="{F7CD77B8-5717-48A5-9E25-F0A154195DAE}"/>
-    <hyperlink ref="T124" r:id="rId110" xr:uid="{5870EC70-AFC1-4984-B63C-70E52D1997C7}"/>
-    <hyperlink ref="T123" r:id="rId111" xr:uid="{2FE6564C-E9AF-47B3-BC71-8D3F9604053F}"/>
-    <hyperlink ref="T127" r:id="rId112" xr:uid="{CB253886-C65A-44AD-83AA-4CB9936DC0E9}"/>
-    <hyperlink ref="T142" r:id="rId113" xr:uid="{8FD3C9C1-19DD-4DE4-BFED-40C1EDDB16F1}"/>
-    <hyperlink ref="B126" r:id="rId114" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/283624f3-e567-4929-b8bc-d33a9f46ea1e" xr:uid="{FC91E404-A8D6-4EA7-B93E-83446233E670}"/>
-    <hyperlink ref="T126" r:id="rId115" xr:uid="{27456D55-2F72-404D-9C8B-C854698E9165}"/>
-    <hyperlink ref="B125" r:id="rId116" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6a792d2d-ca50-468a-9456-895d03fadfd6" xr:uid="{D4243DDC-749D-4275-B355-E031B567E956}"/>
-    <hyperlink ref="T125" r:id="rId117" xr:uid="{081DB7BB-6798-4BBA-9CAC-132A641DD637}"/>
-    <hyperlink ref="B128" r:id="rId118" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6e06488a-6cb6-428b-9ed6-c8c73ef8b763" xr:uid="{870C6C52-B6E1-4366-9D24-2C1E9D97B15C}"/>
-    <hyperlink ref="B129" r:id="rId119" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6e06488a-6cb6-428b-9ed6-c8c73ef8b763" xr:uid="{0DBE4AED-79C9-4D1F-B6BF-0DF81DB8A6E6}"/>
-    <hyperlink ref="T128" r:id="rId120" xr:uid="{E438F1A1-1B16-4AA3-9219-689FFA1E87CB}"/>
-    <hyperlink ref="T129" r:id="rId121" xr:uid="{25B0C20B-7FC6-45F5-9CF8-EA12B3A78096}"/>
-    <hyperlink ref="B133" r:id="rId122" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/4a7d9c16-ca7f-44aa-a2ef-4239c50d26cc" display="Cbus Advocacy Research Survey - Reminder" xr:uid="{56014A37-0DA9-4BC2-A690-FC44626B215E}"/>
-    <hyperlink ref="T133" r:id="rId123" xr:uid="{084B1D27-4465-483D-85B0-F28273391DB3}"/>
-    <hyperlink ref="B139" r:id="rId124" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/92edf682-d87c-422d-8e7b-bb7d146dc839" xr:uid="{E6EF1D18-86DA-462F-B890-F8805E20CCE5}"/>
-    <hyperlink ref="T139" r:id="rId125" xr:uid="{20B61D8D-19A7-4A3E-A798-10CEE9AEF74B}"/>
-    <hyperlink ref="B137" r:id="rId126" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bc71c7b3-ef48-4aba-ad95-ac8cb9712109" xr:uid="{A22BAA73-5D18-498B-901E-BDD442AEF8DC}"/>
-    <hyperlink ref="B138" r:id="rId127" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bc71c7b3-ef48-4aba-ad95-ac8cb9712109" xr:uid="{1080EF57-D511-42D8-BBD2-1077C17CE1D8}"/>
-    <hyperlink ref="T138" r:id="rId128" xr:uid="{DC7BC730-9C8E-42AB-B523-E4F558909582}"/>
-    <hyperlink ref="T137" r:id="rId129" xr:uid="{EE104E06-0CE6-4434-87A1-BE63E2EC99FD}"/>
-    <hyperlink ref="B144" r:id="rId130" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/39dddfa5-71d3-4db1-89ec-f3482f49b94b" xr:uid="{40523AEF-4573-476A-BF62-104B9F750959}"/>
-    <hyperlink ref="B143" r:id="rId131" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/39dddfa5-71d3-4db1-89ec-f3482f49b94b" xr:uid="{1CF92908-8F0B-478A-A7E0-2E0D1F9C7B4F}"/>
-    <hyperlink ref="T144" r:id="rId132" xr:uid="{85D8ACF6-EC7B-484B-9BEC-B0E24AEFDE3B}"/>
-    <hyperlink ref="T143" r:id="rId133" xr:uid="{8ADCB61D-1BA4-4E3A-B2B6-624284BAD8AF}"/>
-    <hyperlink ref="B10" r:id="rId134" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{28B25AE9-4F7D-4F1B-9862-3D666289805E}"/>
-    <hyperlink ref="B8" r:id="rId135" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{AA7C2E3C-4422-4951-8708-469C474A105B}"/>
-    <hyperlink ref="B145" r:id="rId136" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" xr:uid="{A11CCE1F-CB08-4EF8-8E6D-31B3422A7288}"/>
-    <hyperlink ref="B146" r:id="rId137" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" xr:uid="{DCE34DA4-0432-4EDF-9782-2526B7BF935B}"/>
-    <hyperlink ref="B152" r:id="rId138" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 57 Years - Automated Sep Report" xr:uid="{1832F64D-AA22-48DF-AC5C-5140E44E7706}"/>
-    <hyperlink ref="B151" r:id="rId139" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 57 Years - Automated Sep Report" xr:uid="{5551D050-087E-4390-B182-1616970EBD76}"/>
-    <hyperlink ref="B150" r:id="rId140" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 57 Years - Automated Sep Report" xr:uid="{E4B7E407-4979-4D35-B801-225F790EB799}"/>
-    <hyperlink ref="B149" r:id="rId141" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{CAAF221F-68B7-4199-A185-2DFB46FF1094}"/>
-    <hyperlink ref="T152" r:id="rId142" xr:uid="{D9BF2647-E109-4CB9-81F1-ECD9D09437EB}"/>
-    <hyperlink ref="T151" r:id="rId143" xr:uid="{2A3BE898-28E3-468E-A841-818E5F0AC324}"/>
-    <hyperlink ref="T149" r:id="rId144" xr:uid="{D1171090-F3DC-47A0-9B84-7511891F333E}"/>
-    <hyperlink ref="T150" r:id="rId145" xr:uid="{1C6F57FC-CDBA-4341-9E63-EE9913F028E3}"/>
-    <hyperlink ref="B141" r:id="rId146" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{E9FC87C5-54F7-4CB8-A7F8-DDFE177EAD5D}"/>
-    <hyperlink ref="B140" r:id="rId147" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{7F2080F1-684A-44B5-AEDD-4D722FE1D052}"/>
-    <hyperlink ref="B18" r:id="rId148" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{27E0F2FA-FCF6-4E8E-B98F-EF542BEBBEF3}"/>
-    <hyperlink ref="B16" r:id="rId149" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{2D35048C-FB26-4FC3-AD9B-C97FE93800FE}"/>
-    <hyperlink ref="B64" r:id="rId150" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{EB3AA57A-A898-4CA4-B7CE-499CA3EFE349}"/>
-    <hyperlink ref="B62" r:id="rId151" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{D41E71F9-B333-4537-B969-C54B32BAE73F}"/>
-    <hyperlink ref="B113" r:id="rId152" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{EB538D88-BD66-4D15-8B44-94A62534326E}"/>
-    <hyperlink ref="B111" r:id="rId153" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{F66AD42F-5AC0-484A-B6EA-FAD1DA7827F8}"/>
-    <hyperlink ref="B56" r:id="rId154" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{42560414-F49E-43C7-8271-AF9D9065FC22}"/>
-    <hyperlink ref="B55" r:id="rId155" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{630C694F-30D3-49D8-901D-9014C09E771E}"/>
-    <hyperlink ref="B108" r:id="rId156" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{4C5DDE7F-9FA5-4B76-A6CD-769F71F5FD65}"/>
-    <hyperlink ref="B106" r:id="rId157" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{B9C8B1AB-780B-4793-9196-135A5E0C864A}"/>
-    <hyperlink ref="B19" r:id="rId158" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{12E37414-18DA-4186-953F-E5BB530749D2}"/>
-    <hyperlink ref="B17" r:id="rId159" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{CC6FF5ED-2C39-4774-8245-22A540324AF4}"/>
-    <hyperlink ref="B65" r:id="rId160" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{3F5521B6-AE14-4530-8B2D-098986E3A2B6}"/>
-    <hyperlink ref="B63" r:id="rId161" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{9859A856-288D-4DBC-8259-0125513EFDD6}"/>
-    <hyperlink ref="B114" r:id="rId162" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{DB4E5029-79AB-4B71-BB4B-DA93872E2665}"/>
-    <hyperlink ref="B112" r:id="rId163" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{4EB3C59B-5AB6-4FF8-B394-0FBEACB9DDAE}"/>
-    <hyperlink ref="B23" r:id="rId164" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{8BDBBCFB-BFC4-4713-A665-959D3FD8D405}"/>
-    <hyperlink ref="B21" r:id="rId165" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{125CAE76-D66F-46FB-B45A-FC734E3F3C0F}"/>
-    <hyperlink ref="B22" r:id="rId166" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{3619D2E3-049C-495C-99BB-B7C888CBD763}"/>
-    <hyperlink ref="B20" r:id="rId167" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{1D577D2E-861C-4F9B-B487-F3C44378483F}"/>
-    <hyperlink ref="B69" r:id="rId168" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{A5D81D22-5636-4694-8806-92C57FC44478}"/>
-    <hyperlink ref="B67" r:id="rId169" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{23943098-0279-488F-824B-7FBEBCADBD15}"/>
-    <hyperlink ref="B68" r:id="rId170" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{D5B8960F-D042-464A-9468-EE2A6715192E}"/>
-    <hyperlink ref="B66" r:id="rId171" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{7BF59EAE-4D48-4039-9E0B-0DFB48AB37AF}"/>
-    <hyperlink ref="B118" r:id="rId172" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{2B962197-19D1-46CC-9BAF-5E58E2AB29B2}"/>
-    <hyperlink ref="B116" r:id="rId173" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{EDE737E6-545A-4CDA-A2C9-5AAA815C1912}"/>
-    <hyperlink ref="B117" r:id="rId174" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{5C87BAEB-6361-4F87-84AE-35BB546650AA}"/>
-    <hyperlink ref="B115" r:id="rId175" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{6DE5DBBD-4BC9-44A4-B8A1-2CF44A270889}"/>
-    <hyperlink ref="B15" r:id="rId176" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{4E214E15-DE76-4DFE-9E45-6AD2D4EB2924}"/>
-    <hyperlink ref="B14" r:id="rId177" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{AED23E82-24D9-4339-8455-882C9F4B745E}"/>
-    <hyperlink ref="B61" r:id="rId178" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 73 yrs - Automated July Report" xr:uid="{0BFB927B-249A-4940-A13D-459D0CEDCFCC}"/>
-    <hyperlink ref="B60" r:id="rId179" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 55 yrs - Automated July Report" xr:uid="{441AFB7D-5AC3-460E-9FDB-A402F12EA1F9}"/>
-    <hyperlink ref="B110" r:id="rId180" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 73 yrs - Automated July Report" xr:uid="{99C1F603-EAF1-42FF-B65D-AA1818836699}"/>
-    <hyperlink ref="B109" r:id="rId181" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 55 yrs - Automated July Report" xr:uid="{FE3BD79E-85F1-491C-8D3E-1034584CB3F9}"/>
-    <hyperlink ref="B12" r:id="rId182" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" xr:uid="{B1FAE406-F381-468A-A121-6A14BFBBC2B4}"/>
-    <hyperlink ref="B11" r:id="rId183" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{15C78881-B4D5-4750-85F7-75235480710A}"/>
-    <hyperlink ref="B13" r:id="rId184" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{B2C0EA31-5D5E-4F34-8222-B138CD8575F3}"/>
-    <hyperlink ref="B58" r:id="rId185" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{FB526AFF-EB93-4185-BEAD-58B030C61417}"/>
-    <hyperlink ref="B57" r:id="rId186" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{1B22B47B-D362-437F-B489-CDB4A84B1907}"/>
-    <hyperlink ref="B59" r:id="rId187" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{C05B998E-F0FE-496D-B2C8-450D8EB2672F}"/>
-    <hyperlink ref="B9" r:id="rId188" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" display="Beneficiaries [Seg 4 - Lapsed binding] - Automated July Report" xr:uid="{0CA9DB7A-5DE6-452A-8CB3-F20C06315E06}"/>
-    <hyperlink ref="B107" r:id="rId189" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" display="Beneficiaries [Seg 4 - Lapsed binding] - Automated July Report" xr:uid="{29BA7AE2-D727-48C5-8BB6-F40AEBA48DDC}"/>
-    <hyperlink ref="B6" r:id="rId190" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df53f790-6392-4a01-a73f-f23a41796609" display="PYS 12 Months - Automated July Report" xr:uid="{B8C16EF4-1EB0-439E-9931-8CCBEBB7434F}"/>
-    <hyperlink ref="B7" r:id="rId191" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df53f790-6392-4a01-a73f-f23a41796609" display="PYS 12 Months - Automated July Report" xr:uid="{F8F9A670-BB32-4D63-A566-5C5D144A68A4}"/>
-    <hyperlink ref="B129:B132" r:id="rId192" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df53f790-6392-4a01-a73f-f23a41796609" display="PYS 12 Months - Automated July Report" xr:uid="{5A57F3AC-8F37-4AA2-AEC3-D228861D25E1}"/>
-    <hyperlink ref="B5" r:id="rId193" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" display="SPC" xr:uid="{BE4B61FC-D27B-4CD6-9DCB-597D9B237175}"/>
-    <hyperlink ref="B52" r:id="rId194" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" display="SPC" xr:uid="{7C1DD57D-0992-4981-92FB-393607C4E760}"/>
-    <hyperlink ref="B103" r:id="rId195" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" display="SPC" xr:uid="{4724CBB6-757A-4570-AC13-3FD363F876BC}"/>
-    <hyperlink ref="B2" r:id="rId196" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" xr:uid="{FC6E80E8-E09B-4E1C-800C-92FA7943F72B}"/>
-    <hyperlink ref="B137:B138" r:id="rId197" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" display="Abandoned  Cart MJOL" xr:uid="{89E7B679-7362-475D-98BE-25F1829C350A}"/>
-    <hyperlink ref="T18" r:id="rId198" xr:uid="{1ABD2676-EB8A-4847-847A-4104CD4746DF}"/>
-    <hyperlink ref="B147" r:id="rId199" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bd610eaf-020d-4ee0-8920-be3e08a37a25" xr:uid="{DEABCB06-B632-461D-84C6-F06A70FA9619}"/>
-    <hyperlink ref="B148" r:id="rId200" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3df19f42-c622-481a-a0cc-b64ea8f94164" display="Cbus - 2025 Statements - SIS" xr:uid="{8C7106E8-B2C7-4073-98E2-6BD22D598D4F}"/>
-    <hyperlink ref="T148" r:id="rId201" xr:uid="{46704411-4366-4503-871A-63C62D6F5CDF}"/>
-    <hyperlink ref="T147" r:id="rId202" xr:uid="{35617BE4-D51B-4C42-BCBC-A3326810417E}"/>
-    <hyperlink ref="B153" r:id="rId203" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df121502-9927-4eed-8a89-998f44dfe2cb" xr:uid="{4C7035C0-55DC-42DB-BC1A-1724968D036A}"/>
-    <hyperlink ref="B154" r:id="rId204" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df121502-9927-4eed-8a89-998f44dfe2cb" xr:uid="{D51BF1B3-CB4F-4C37-97E4-0E8A747D3371}"/>
-    <hyperlink ref="T153" r:id="rId205" xr:uid="{6D9DC780-9CDA-4D3F-B56F-0677CA3C5FB2}"/>
-    <hyperlink ref="T154" r:id="rId206" xr:uid="{E660BB65-5617-4FC2-B761-2C921DC44FB7}"/>
-    <hyperlink ref="B120" r:id="rId207" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{787E3B42-1A34-460D-BCBD-6D1DEBA1028A}"/>
-    <hyperlink ref="B119" r:id="rId208" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" xr:uid="{CAB5B92A-46CB-4743-B631-1BDD2851A0CE}"/>
-    <hyperlink ref="B71" r:id="rId209" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{95384588-A5DD-422B-8251-86A1E34F35E7}"/>
-    <hyperlink ref="B70" r:id="rId210" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{690ACB40-AD80-4398-88D6-EF31DB93FD07}"/>
-    <hyperlink ref="B25" r:id="rId211" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{ACA5534A-56E5-44DB-8EBF-E9C689DD70E6}"/>
-    <hyperlink ref="B24" r:id="rId212" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{8FEB3484-B05E-47F9-99FD-554CD58C3EA1}"/>
-    <hyperlink ref="B122" r:id="rId213" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" xr:uid="{403A0435-2A6E-4B4F-AB1E-59A9DD3D7421}"/>
-    <hyperlink ref="B121" r:id="rId214" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" xr:uid="{70EDC27F-2DC1-4DB6-8815-947052CC4758}"/>
-    <hyperlink ref="B73" r:id="rId215" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" display="6 Month Tenure [Pre 17 Sep 2025]" xr:uid="{BAACE1B3-18DD-40D4-B9D4-9C9FFC7032EA}"/>
-    <hyperlink ref="B72" r:id="rId216" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" display="6 Month Tenure [Pre 17 Sept 2025]" xr:uid="{90BD2120-2520-423A-878B-E4198EC602E4}"/>
-    <hyperlink ref="B153:B154" r:id="rId217" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" display="6 Month Tenure [Pre 17 Sept 2025]" xr:uid="{011C95CE-D787-4DFF-A58A-52BB55F1A47F}"/>
-    <hyperlink ref="B157" r:id="rId218" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{95F5B5C6-E7F9-4F03-BCC3-72C6C47E693A}"/>
-    <hyperlink ref="B158" r:id="rId219" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{0A3ED4AD-923A-41AB-8AA4-552B42BFBC3C}"/>
-    <hyperlink ref="B159" r:id="rId220" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{9CD36ECF-BF41-4F3E-9C75-670618C667D2}"/>
-    <hyperlink ref="B160" r:id="rId221" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{3851E138-F07F-4299-82F1-CDACC7AB2D4F}"/>
-    <hyperlink ref="T157" r:id="rId222" xr:uid="{F2675824-1A9F-49D9-A78F-51A609CB7E9D}"/>
-    <hyperlink ref="T158" r:id="rId223" xr:uid="{76235692-6651-4E03-9AAE-80F4C54EA185}"/>
-    <hyperlink ref="T160" r:id="rId224" xr:uid="{B292C362-9C06-4B60-942C-245AE8714903}"/>
-    <hyperlink ref="T159" r:id="rId225" xr:uid="{EF137438-E2BA-480C-9EEA-2E208B2FF391}"/>
-    <hyperlink ref="B156" r:id="rId226" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{594850D2-A800-4945-A1A3-7601E7DFC5BA}"/>
-    <hyperlink ref="B155" r:id="rId227" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{B56A7C75-F3A7-41B8-AB09-941E011BBE2B}"/>
-    <hyperlink ref="B161" r:id="rId228" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{EC7A412D-E0CD-473A-92EC-8B71EC598FC0}"/>
-    <hyperlink ref="B162" r:id="rId229" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{5B6183F1-E7D9-4E23-8A1E-85D2D04FC441}"/>
-    <hyperlink ref="B163" r:id="rId230" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{B402C10B-4B83-4737-83E5-8CFA813ECEB4}"/>
-    <hyperlink ref="B164" r:id="rId231" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{37A7B1A0-5954-4F69-A396-24AAA969F4E7}"/>
-    <hyperlink ref="B165" r:id="rId232" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{B18BF7CB-5575-459F-973A-30561B8958FE}"/>
-    <hyperlink ref="B166" r:id="rId233" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{9D326E37-133E-4777-A180-AD1C95B3D1D2}"/>
-    <hyperlink ref="B167" r:id="rId234" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{F245AA5F-1AE2-4629-900B-0CB71BF249ED}"/>
-    <hyperlink ref="B168" r:id="rId235" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{D5E69B1E-2DD7-48B4-A931-6A46F1D52FE4}"/>
-    <hyperlink ref="B169" r:id="rId236" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{AE17125C-908A-451D-BAB3-78150075D391}"/>
-    <hyperlink ref="B170" r:id="rId237" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{FCDBE11B-CC1D-44AE-BAC3-6BF06E4A6EEB}"/>
-    <hyperlink ref="B171" r:id="rId238" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{F6A1F5A1-0BCA-4C33-AB46-BD7106ACD0A6}"/>
-    <hyperlink ref="B172" r:id="rId239" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{5D070645-C605-48A6-B30A-545539E44075}"/>
-    <hyperlink ref="B173" r:id="rId240" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" xr:uid="{3D07B372-B516-4FA3-97CF-D7FA84A3AC31}"/>
-    <hyperlink ref="B176" r:id="rId241" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" xr:uid="{F0EF1DE0-C482-4FE6-A769-98A5CF368ADF}"/>
-    <hyperlink ref="B178" r:id="rId242" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" display="6 Month Tenure [Pre 17 Sep 2025]" xr:uid="{560F601D-574D-4934-AD09-006713AC4CDC}"/>
-    <hyperlink ref="B186" r:id="rId243" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{96C74F20-FE6A-40F8-AA31-5644008F3617}"/>
-    <hyperlink ref="T186" r:id="rId244" xr:uid="{D8F82DA6-CC4A-493E-A6B4-B86927821944}"/>
-    <hyperlink ref="B187" r:id="rId245" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{B1D0FF54-7018-42C6-B8F9-A5E1BF28F722}"/>
-    <hyperlink ref="T187" r:id="rId246" xr:uid="{6AE8FEA1-47CB-4F24-B9A5-5E882E21AC38}"/>
-    <hyperlink ref="B188" r:id="rId247" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{8A9343BC-24AB-4F65-8509-CA061FD69388}"/>
-    <hyperlink ref="T188" r:id="rId248" xr:uid="{93AFC6AB-9BA1-4973-92F3-F790ACDE4D19}"/>
-    <hyperlink ref="B189" r:id="rId249" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{14E99629-55BD-48C9-B1BA-1FDF579A92AE}"/>
-    <hyperlink ref="T189" r:id="rId250" xr:uid="{03849D1B-E17B-4AD6-B577-6CF3F1BBB6CD}"/>
-    <hyperlink ref="B191" r:id="rId251" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b3c83ca1-5def-411e-8a8a-b1fa4230bca9" xr:uid="{212C918E-50B9-4332-B1C2-01AD126D7D41}"/>
-    <hyperlink ref="B190" r:id="rId252" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b3c83ca1-5def-411e-8a8a-b1fa4230bca9" xr:uid="{747F800E-4385-4B16-AF7F-18B7A6E1DCBA}"/>
-    <hyperlink ref="B177" r:id="rId253" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" xr:uid="{D2BB8B2B-A730-4842-96DA-050B58161FA7}"/>
-    <hyperlink ref="B193" r:id="rId254" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/11c7ab80-6498-486d-8799-60566311d059" xr:uid="{D028E486-7C5C-4F19-BC7C-4D0BF4854C81}"/>
-    <hyperlink ref="B194" r:id="rId255" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/11c7ab80-6498-486d-8799-60566311d059" xr:uid="{EC080CCE-4AC3-44C9-846F-24E8A6E373E2}"/>
-    <hyperlink ref="B198" r:id="rId256" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{D18EE3B5-4079-4B25-85C7-EED23D580736}"/>
-    <hyperlink ref="B197" r:id="rId257" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" display="Advice Needs research" xr:uid="{102FCE9B-70AE-41E5-87B2-139F4ABCDDFC}"/>
-    <hyperlink ref="B199" r:id="rId258" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{3FE70EE3-023F-4E4B-BBF2-78E8EA52A0B4}"/>
-    <hyperlink ref="B200" r:id="rId259" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e72ad46a-3745-40ba-a629-d9f53273a656" display="Scam awareness EDM" xr:uid="{8AF7365D-29AF-42A6-B6EF-DE0F6A74D90E}"/>
-    <hyperlink ref="B201" r:id="rId260" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e72ad46a-3745-40ba-a629-d9f53273a656" display="Scam awareness EDM" xr:uid="{810FFCD4-E9A1-4CA2-BE71-0B3F9838A0F3}"/>
-    <hyperlink ref="B180" r:id="rId261" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{EC52EDA4-B983-4691-994A-4372BFCF8AB8}"/>
-    <hyperlink ref="B181" r:id="rId262" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{2F265E0D-9A04-4F85-9612-18A7045D0D63}"/>
-    <hyperlink ref="B182" r:id="rId263" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{72F11345-FB57-4891-AFCB-A7021674E90D}"/>
-    <hyperlink ref="B183" r:id="rId264" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{20208A02-C4B2-4288-907A-1191A7C238BE}"/>
-    <hyperlink ref="B179" r:id="rId265" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" display="6 Month Tenure [Pre 17 Sep 2025]" xr:uid="{AABAB842-6D2C-4F7E-85C6-832CD62AC046}"/>
-    <hyperlink ref="B202" r:id="rId266" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/dd583dec-4a8f-4364-b58b-eeb1bca64b4d" xr:uid="{B7F0A43A-9F04-440F-AD9C-9105037D6F5C}"/>
-    <hyperlink ref="B203" r:id="rId267" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/dd583dec-4a8f-4364-b58b-eeb1bca64b4d" xr:uid="{DD788B99-0528-4A31-9DA2-3F14526C441E}"/>
-    <hyperlink ref="B204" r:id="rId268" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1705c74b-00e3-4f10-ba53-8d31b070761f" xr:uid="{17785F7D-009F-47E5-BBC0-003E27DEA98B}"/>
-    <hyperlink ref="B205" r:id="rId269" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1705c74b-00e3-4f10-ba53-8d31b070761f" xr:uid="{D3C43F25-13E2-464D-BC6A-ACA9A0C7C58D}"/>
-    <hyperlink ref="T206" r:id="rId270" xr:uid="{8BE67F82-F3D7-4965-828D-53844EB241DB}"/>
-    <hyperlink ref="T207" r:id="rId271" xr:uid="{F7ECDDC4-C378-4C02-ADFF-9C619DE281B0}"/>
-    <hyperlink ref="T208" r:id="rId272" xr:uid="{DE67BC14-DC57-4C4C-8FE5-3ACFBDA435C4}"/>
-    <hyperlink ref="T217" r:id="rId273" xr:uid="{C7E19626-02A4-4B0C-B60E-86E179849241}"/>
-    <hyperlink ref="T216" r:id="rId274" xr:uid="{D891EFB4-ACAF-45AA-832E-A8B62891E532}"/>
-    <hyperlink ref="T209" r:id="rId275" xr:uid="{308B7210-80CE-4BFD-9B40-FDB3B1E0E14D}"/>
-    <hyperlink ref="T210" r:id="rId276" xr:uid="{5D44B1DF-075A-4461-BA16-F256BCB5DB2F}"/>
-    <hyperlink ref="T211" r:id="rId277" xr:uid="{AC14882E-C08F-418B-89F1-712D6C01D1EB}"/>
-    <hyperlink ref="T212" r:id="rId278" xr:uid="{D65178F1-7C36-4856-968B-BB7AFA21409D}"/>
-    <hyperlink ref="T213" r:id="rId279" xr:uid="{B27A6DAE-AEF7-4B53-BFDF-7010146F131A}"/>
-    <hyperlink ref="T214" r:id="rId280" xr:uid="{8190AD1D-5D8B-4E66-B390-2F27A170F62F}"/>
-    <hyperlink ref="T215" r:id="rId281" xr:uid="{1A1D7CA3-25FC-465E-8689-45457A25D40D}"/>
-    <hyperlink ref="B218" r:id="rId282" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{E1872C75-D226-47E3-AF54-1A01D18B09E6}"/>
-    <hyperlink ref="B219" r:id="rId283" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{3461D3D2-9801-47C0-BE04-13C65711D695}"/>
-    <hyperlink ref="B220" r:id="rId284" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{D4B47714-368B-4369-BC6A-CE3BF62714B4}"/>
-    <hyperlink ref="B221" r:id="rId285" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{530F7378-391C-4B8F-ABC0-9D46F6F0F7C4}"/>
-    <hyperlink ref="B222" r:id="rId286" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{05123249-3A00-4E04-9FA3-0FAF2BC645C5}"/>
-    <hyperlink ref="B223" r:id="rId287" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{9EDD1503-471B-46D8-A716-808692FB771A}"/>
-    <hyperlink ref="B224" r:id="rId288" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{F57197D2-BDF7-4008-AFD0-70B7D9715401}"/>
-    <hyperlink ref="B225" r:id="rId289" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{9CACDA5D-7A93-4498-910D-CB23E2DD242F}"/>
-    <hyperlink ref="B226" r:id="rId290" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" xr:uid="{9AAA07F3-02AF-4AF9-976C-35C0B3FBDD69}"/>
-    <hyperlink ref="B229" r:id="rId291" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" xr:uid="{60B4CB47-B5E1-4484-AB18-9847FCCFAFF2}"/>
-    <hyperlink ref="B230" r:id="rId292" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" xr:uid="{95C6780C-2B2D-4C98-8481-E4E825CBE9BF}"/>
-    <hyperlink ref="B231" r:id="rId293" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{0021A7F2-DD1B-4870-9404-16898343915B}"/>
-    <hyperlink ref="B232" r:id="rId294" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{53DF61B3-616E-480C-9213-CCC9AC61DF56}"/>
-    <hyperlink ref="B233" r:id="rId295" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{E79F2A25-E7F2-40DB-926C-4F4EB6753687}"/>
-    <hyperlink ref="B234" r:id="rId296" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{DFEB8853-4230-4E7F-84A7-0B899306326B}"/>
-    <hyperlink ref="B227:B228" r:id="rId297" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e1d432aa-88e8-4c3a-89bb-7cfed646e1be" display="PYS 12 Months" xr:uid="{2704B708-84EA-4C85-8C04-062100C8F184}"/>
-    <hyperlink ref="B235" r:id="rId298" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{4C0A1E69-2558-4BB8-B21B-397325219DC8}"/>
-    <hyperlink ref="B236" r:id="rId299" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{76AAD98C-AAC2-4503-AA34-8B434EE3ED3E}"/>
-    <hyperlink ref="B238" r:id="rId300" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{FC9C2CA8-8ABC-4F1E-BB1E-03A815CF8CD8}"/>
-    <hyperlink ref="B237" r:id="rId301" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{8838D11D-6FBD-48CF-9CA4-EDBB1F82F383}"/>
-    <hyperlink ref="B185" r:id="rId302" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{B7867DAB-269E-4524-91A1-534B6EDD7C51}"/>
-    <hyperlink ref="B184" r:id="rId303" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{9D599D62-17C9-498F-8055-4133593F374D}"/>
-    <hyperlink ref="B239" r:id="rId304" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/854f73d8-aa00-4fe2-9c2e-45bcb54156f4" xr:uid="{C1027C14-56EA-448E-8BAB-C63E09D0C9E4}"/>
-    <hyperlink ref="B240" r:id="rId305" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/854f73d8-aa00-4fe2-9c2e-45bcb54156f4" xr:uid="{384E04F6-4003-476E-B192-E063148EA31B}"/>
-    <hyperlink ref="B242" r:id="rId306" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{02010B3C-9466-465E-936C-9470E6B34533}"/>
-    <hyperlink ref="B241" r:id="rId307" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" display="Advice Needs research" xr:uid="{AE77844B-C2CD-4063-8DD4-6E106784FF21}"/>
-    <hyperlink ref="B243" r:id="rId308" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{2E8F6402-4182-4DDE-A83F-CCF9127227F3}"/>
-    <hyperlink ref="B241:B243" r:id="rId309" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/09bbe6ac-c38b-4e06-9ae0-fa2b7779445b" display="Advice Needs research- MEDIA 35s+ Reminder" xr:uid="{B63A33C9-482B-449F-9AF5-9895152EAB9F}"/>
-    <hyperlink ref="B244" r:id="rId310" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/51b42ebc-0a9a-4491-a1fa-669bce1a67e7" display="YC Investment Basics" xr:uid="{47D98467-B2C4-4A72-B0B6-64FB8BC26859}"/>
-    <hyperlink ref="B245:B247" r:id="rId311" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/51b42ebc-0a9a-4491-a1fa-669bce1a67e7" display="YC Investment Basics" xr:uid="{5F39ABA6-87A9-4E9D-A6EE-905C88ABE4DF}"/>
-    <hyperlink ref="T244" r:id="rId312" xr:uid="{18314DDC-5F4F-4BDB-A668-B5872785532C}"/>
-    <hyperlink ref="T245" r:id="rId313" xr:uid="{7BADFD5C-DAEF-4DE1-A527-593BE81D4E72}"/>
-    <hyperlink ref="T246" r:id="rId314" xr:uid="{F7E6F66E-D9EA-4898-900D-5532E4671623}"/>
-    <hyperlink ref="T247" r:id="rId315" xr:uid="{5A74C3FC-5D44-4CFB-89D8-A45337A2B428}"/>
-    <hyperlink ref="B248" r:id="rId316" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3e292887-b584-4bcf-8302-372f4e8f75d2" xr:uid="{F6016358-C5B9-40C3-96F3-C601559DB907}"/>
-    <hyperlink ref="B249" r:id="rId317" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/98bceed7-967d-4787-a4c1-29e5d4f011c6" display="Quarterly Investment Perf Update - HNW" xr:uid="{1A2508D2-E90A-4CBB-8B8C-963174C904B8}"/>
-    <hyperlink ref="B250" r:id="rId318" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/98bceed7-967d-4787-a4c1-29e5d4f011c6" display="Quarterly Investment Perf Update - HNW" xr:uid="{0AA40987-2B11-42F9-81C9-236D7843AC8D}"/>
-    <hyperlink ref="T249" r:id="rId319" xr:uid="{D97EE891-4645-49D2-B25F-26C14EFC3BEF}"/>
-    <hyperlink ref="T250" r:id="rId320" xr:uid="{13D1D080-A49D-42A1-8A13-AC04792EAEEB}"/>
-    <hyperlink ref="B251" r:id="rId321" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b2d213d8-d137-4f0b-bd6c-535471820e6f" xr:uid="{0C3F0A6D-5EE8-4501-803F-ADDCAD0ED220}"/>
-    <hyperlink ref="B252" r:id="rId322" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b2d213d8-d137-4f0b-bd6c-535471820e6f" xr:uid="{38CF9644-43F9-483B-886E-9A492D9C3A3B}"/>
-    <hyperlink ref="T251" r:id="rId323" xr:uid="{678283B0-C9B8-42D6-88C9-59FCE516EEB7}"/>
-    <hyperlink ref="T252" r:id="rId324" xr:uid="{F2DBCCEF-744E-4DBE-9BC8-6CD22C6569A1}"/>
-    <hyperlink ref="B253" r:id="rId325" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f4685d9b-1aa1-48e0-88a5-676af16225cf" xr:uid="{9AB60A34-75B2-46E6-867A-C6D18F6473D8}"/>
-    <hyperlink ref="B254" r:id="rId326" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f4685d9b-1aa1-48e0-88a5-676af16225cf" xr:uid="{6EBAF5FD-971F-43EB-BC02-D9DED04180AA}"/>
-    <hyperlink ref="T253" r:id="rId327" xr:uid="{EF9898B8-4752-4803-84B4-723099440F4F}"/>
-    <hyperlink ref="T254" r:id="rId328" xr:uid="{2C97B4E3-E071-4FC9-8214-2E7EFF682463}"/>
-    <hyperlink ref="B255" r:id="rId329" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6a9f570b-c2e8-4903-8f56-8a02b73a7926" xr:uid="{6F27F4B5-83E3-4C53-BCB6-11143FEAB1D0}"/>
-    <hyperlink ref="B256" r:id="rId330" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6a9f570b-c2e8-4903-8f56-8a02b73a7926" display="SEN - Death Benefit Nov 25" xr:uid="{D7AAF38C-5652-4386-8A71-3DA5707467F1}"/>
-    <hyperlink ref="T255" r:id="rId331" xr:uid="{3E8DCB2C-2CBD-444A-AE77-A07E924D1512}"/>
-    <hyperlink ref="T256" r:id="rId332" xr:uid="{9A418F6D-2E11-4129-8625-EBA8CBF24892}"/>
-    <hyperlink ref="T257" r:id="rId333" xr:uid="{8D57081E-13DF-438D-889C-CE6E066BDC9C}"/>
-    <hyperlink ref="B258" r:id="rId334" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{A194A329-BFAE-4C41-A6E8-5281732B1448}"/>
+    <hyperlink ref="B32" r:id="rId1" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{7F7AB8F8-DEAF-3449-99E1-B7BA87B8D6EF}"/>
+    <hyperlink ref="B33" r:id="rId2" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{B63C576D-7994-6D43-BAC0-C9CB36419E3D}"/>
+    <hyperlink ref="B28" r:id="rId3" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{55F1AE99-10CB-7148-815A-490ABAE8C7E5}"/>
+    <hyperlink ref="B29" r:id="rId4" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{E086D344-6939-0546-BD48-E1DE212F93A3}"/>
+    <hyperlink ref="B30" r:id="rId5" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{BA7A759B-B2FB-C64C-AACF-2D62F08DC76A}"/>
+    <hyperlink ref="B31" r:id="rId6" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{4D168887-CA13-A245-A790-692A0821F674}"/>
+    <hyperlink ref="B34" r:id="rId7" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{A74DA7AF-FF8B-CD43-A7F7-7E57FBD2A7BA}"/>
+    <hyperlink ref="B35" r:id="rId8" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{0DCFFBD3-AB88-B84D-96F9-F86FD4E67D64}"/>
+    <hyperlink ref="B37" r:id="rId9" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{6DF15277-6029-7343-8803-C69575ED3570}"/>
+    <hyperlink ref="B36" r:id="rId10" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="EOFY Performance" xr:uid="{4F2D85B6-4267-0641-8B81-5023B9593C70}"/>
+    <hyperlink ref="B38" r:id="rId11" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="EOFY Performance" xr:uid="{B316FBC2-9FEE-B340-A267-E6ECABFCA375}"/>
+    <hyperlink ref="B39" r:id="rId12" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="EOFY Performance" xr:uid="{ED60402C-1452-B241-8941-D6448A79EB4B}"/>
+    <hyperlink ref="B40" r:id="rId13" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{2DDC3489-8245-B045-B27C-0C53BE66B1D3}"/>
+    <hyperlink ref="B41" r:id="rId14" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{CC18B321-7B40-B14C-B0BA-0B394F37FB1B}"/>
+    <hyperlink ref="B42" r:id="rId15" location="/@cbus/sname:prod/journey-optimizer/journey/report/" display="CBUS - Corporate insurance SEN (AME) Cbus" xr:uid="{C540744B-5256-B74D-917A-E9C3183B0ED0}"/>
+    <hyperlink ref="B43" r:id="rId16" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{D2AD9D56-ED8D-A74B-BF75-E0A47B438E34}"/>
+    <hyperlink ref="B44" r:id="rId17" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{E0417873-39DF-B845-B923-0200FA9CA2F7}"/>
+    <hyperlink ref="B49" r:id="rId18" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{D74E4B1C-FE5C-C542-800C-ECA69E65CCF0}"/>
+    <hyperlink ref="B50" r:id="rId19" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{9E4CF538-4AC2-1849-8C5A-4AB7B64B6F63}"/>
+    <hyperlink ref="B45" r:id="rId20" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{B25CC288-D429-7342-8850-3247BA70AFCE}"/>
+    <hyperlink ref="B46" r:id="rId21" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{53BC90F5-EC80-0D48-BDE3-6B226F229779}"/>
+    <hyperlink ref="B47" r:id="rId22" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{9AB33328-4010-F843-B550-8D7E64EC2CD1}"/>
+    <hyperlink ref="B48" r:id="rId23" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{1CD36E2E-A888-B64A-A43F-52462AF0D631}"/>
+    <hyperlink ref="T32" r:id="rId24" xr:uid="{1077084C-D29E-4ABC-BD53-A05F91719125}"/>
+    <hyperlink ref="T33" r:id="rId25" xr:uid="{E82B6BA4-E16F-492E-BCD8-911C556EA12C}"/>
+    <hyperlink ref="T28" r:id="rId26" xr:uid="{6184ED25-1DF9-49D3-AC87-98D010A3B3E0}"/>
+    <hyperlink ref="T29" r:id="rId27" xr:uid="{23489B88-1AF7-440D-82A5-D2C99B402CE1}"/>
+    <hyperlink ref="T30" r:id="rId28" xr:uid="{29D38B7B-0EEB-4F1D-BD67-2FE0B692C886}"/>
+    <hyperlink ref="T31" r:id="rId29" xr:uid="{E529B59E-BC39-41D7-A6B8-B76C65B02964}"/>
+    <hyperlink ref="T34" r:id="rId30" xr:uid="{75D776C4-686E-4764-A0CE-7978746739AA}"/>
+    <hyperlink ref="T35" r:id="rId31" xr:uid="{18534669-D2F7-4C45-BE71-B06E441E98C4}"/>
+    <hyperlink ref="T40" r:id="rId32" xr:uid="{4456DFDD-02ED-4178-A1B2-7A56262C79A7}"/>
+    <hyperlink ref="T41" r:id="rId33" xr:uid="{85BEFFFA-77A3-49CF-94D8-7F3EBFED1A80}"/>
+    <hyperlink ref="T43" r:id="rId34" xr:uid="{9D50E18A-27F4-4E22-95C5-F200362F77FE}"/>
+    <hyperlink ref="T44" r:id="rId35" xr:uid="{49F0C4D7-6B49-48CB-9B69-3680BAAED979}"/>
+    <hyperlink ref="T49" r:id="rId36" xr:uid="{669F8622-A0EA-44FE-8AAA-EAB6EE53AEB9}"/>
+    <hyperlink ref="T50" r:id="rId37" xr:uid="{3EC869FD-833C-4252-AFF2-954077725E77}"/>
+    <hyperlink ref="B74" r:id="rId38" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2b3a8bd7-9314-4486-bed5-590aae72eef6" xr:uid="{DDE7FEFC-6B1E-4AA0-B976-36D2973B650E}"/>
+    <hyperlink ref="T74" r:id="rId39" xr:uid="{7AD33B0E-E2D3-41B8-9172-D15847D781D8}"/>
+    <hyperlink ref="B75" r:id="rId40" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/837cd468-99da-4b6c-86ed-a729c8dedaed" xr:uid="{8D543BC5-E411-41F4-AC77-9D04065517CB}"/>
+    <hyperlink ref="T75" r:id="rId41" xr:uid="{0118962C-499A-4545-8BD4-3ABE37EC8589}"/>
+    <hyperlink ref="B76" r:id="rId42" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1c60eb15-5315-4d97-bc92-f3321a8f2bb8" xr:uid="{0C3ADEAB-E937-4D0F-A344-AB2EAC09C8ED}"/>
+    <hyperlink ref="T76" r:id="rId43" xr:uid="{EA3D39DE-B821-4DE6-A6E8-54C4DB4002CB}"/>
+    <hyperlink ref="B79" r:id="rId44" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d0d232aa-3290-434d-8c3f-c589a73ea607" xr:uid="{21BFCBA6-6AD1-4DF1-BFCC-97AF53BF164E}"/>
+    <hyperlink ref="B80" r:id="rId45" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d0d232aa-3290-434d-8c3f-c589a73ea607" xr:uid="{FFD820BD-0682-4A01-886A-FC6E140DD7F6}"/>
+    <hyperlink ref="T79" r:id="rId46" xr:uid="{BDD938AD-4F2D-4D6D-A609-A2D733A83114}"/>
+    <hyperlink ref="T80" r:id="rId47" xr:uid="{54C0322F-D13C-44D8-B6EB-53DBB2BCA1C8}"/>
+    <hyperlink ref="B77" r:id="rId48" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/10c562f8-f91d-4456-8e2f-4ac211353527" xr:uid="{10A9ABF1-9B48-49EB-8857-3A95282225D7}"/>
+    <hyperlink ref="B78" r:id="rId49" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/10c562f8-f91d-4456-8e2f-4ac211353527" xr:uid="{03BE0AA5-037E-4E17-8386-29BAE9E3BEE5}"/>
+    <hyperlink ref="T77" r:id="rId50" xr:uid="{337F27CF-D0CD-4B04-A48D-36C253F1BE4F}"/>
+    <hyperlink ref="T78" r:id="rId51" xr:uid="{7FE3D493-8D5B-4496-8F77-D73CA4BD72FB}"/>
+    <hyperlink ref="B82" r:id="rId52" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2be0e003-3e51-476c-86ea-8a1f8913d899" xr:uid="{DCBBFEEB-0E31-4647-A7B8-662452421D74}"/>
+    <hyperlink ref="B83" r:id="rId53" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2be0e003-3e51-476c-86ea-8a1f8913d899" xr:uid="{F08C799E-E69A-4FAE-9577-3BE26DC55F8C}"/>
+    <hyperlink ref="T82" r:id="rId54" xr:uid="{F25A322F-4512-4FB9-896D-FC4488D151BC}"/>
+    <hyperlink ref="T83" r:id="rId55" xr:uid="{E9B325CA-DA26-471B-8892-3CD505753BC9}"/>
+    <hyperlink ref="B81" r:id="rId56" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d5aac9ae-16b6-46ce-9310-1ba0004b45ea" xr:uid="{FCD585C4-F8D5-442F-82A2-8DA88F7E9D6B}"/>
+    <hyperlink ref="T81" r:id="rId57" xr:uid="{E2C5678C-A592-4E8F-8D77-8769EA44690D}"/>
+    <hyperlink ref="B84" r:id="rId58" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cb123bc-fd8e-4868-82f1-14995d53c591" xr:uid="{930F7BAC-EDE4-4C25-8B39-8677C9CD53AD}"/>
+    <hyperlink ref="B85" r:id="rId59" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cb123bc-fd8e-4868-82f1-14995d53c591" xr:uid="{DDF5BEEE-A105-4CBA-B3EF-4B0632B51EAE}"/>
+    <hyperlink ref="T84" r:id="rId60" xr:uid="{28F02C08-2175-4786-AE8B-EF7115BB2A13}"/>
+    <hyperlink ref="T85" r:id="rId61" xr:uid="{6B6FA851-5730-41C3-9AD3-29501233C4EF}"/>
+    <hyperlink ref="B86" r:id="rId62" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/47e8e523-4417-4b5b-90e5-f72b14e59a38" display="Cbus Advocacy Research" xr:uid="{415E68FE-63DA-4727-BBF2-D5B9E5B4A68B}"/>
+    <hyperlink ref="T86" r:id="rId63" xr:uid="{2AD3FFE5-FB20-4C1E-B57F-CFE0E5B36B26}"/>
+    <hyperlink ref="B89" r:id="rId64" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/50c38354-a1aa-4221-89a9-67b1c2af5d56" xr:uid="{776AA357-15C0-415F-AD46-2E881767E760}"/>
+    <hyperlink ref="T89" r:id="rId65" xr:uid="{67874548-D942-44D2-AFBC-BB37ACD6D8B7}"/>
+    <hyperlink ref="B87" r:id="rId66" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bcdec3d6-9690-4399-8cce-1c945390b466" xr:uid="{17B72274-B78F-495D-B419-9A0D73821A7F}"/>
+    <hyperlink ref="B88" r:id="rId67" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bcdec3d6-9690-4399-8cce-1c945390b466" xr:uid="{C08F1CF4-F712-4502-B9D7-AB516367C6BC}"/>
+    <hyperlink ref="T87" r:id="rId68" xr:uid="{09AA577A-31BB-4E89-AD1C-E223A35FAD60}"/>
+    <hyperlink ref="T88" r:id="rId69" xr:uid="{720B7893-DA39-46C3-87FA-F12DA6138BED}"/>
+    <hyperlink ref="B92" r:id="rId70" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e48b4e16-bdcf-44b1-87db-8546a575ba4e" display="EOFY investment performance campaign (Microsoft HNW, SIS, Media)" xr:uid="{69BF4C00-E3BA-45B0-811B-3788561FDB24}"/>
+    <hyperlink ref="B91" r:id="rId71" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e48b4e16-bdcf-44b1-87db-8546a575ba4e" display="EOFY investment performance campaign (Microsoft HNW, SIS, Media)" xr:uid="{D7585B4B-7204-4A4E-B140-4217FD309F7E}"/>
+    <hyperlink ref="B90" r:id="rId72" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e48b4e16-bdcf-44b1-87db-8546a575ba4e" display="EOFY investment performance campaign (Microsoft HNW, SIS, Media)" xr:uid="{8256078B-EEC5-4D3C-87D3-6EDECA6A4325}"/>
+    <hyperlink ref="T91" r:id="rId73" xr:uid="{BD617822-7DD4-4BC8-8F4E-3DD549DB69D2}"/>
+    <hyperlink ref="T38" r:id="rId74" xr:uid="{43E542A7-EED9-47CD-A876-76D47F10BB49}"/>
+    <hyperlink ref="B93" r:id="rId75" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/7e56f57e-12e2-49c0-9e51-de68fe9cf789" display="#1 - SIS Acquisition - 2025 AUG" xr:uid="{E1FC8E26-35AB-43CA-8415-357E70A82AA7}"/>
+    <hyperlink ref="B95" r:id="rId76" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bca1837c-0f90-4529-9649-68676fad5162" display="#2 - SIS Acquisition - 2025 AUG" xr:uid="{83A5C014-4EB4-4268-8408-8C349E11D7B2}"/>
+    <hyperlink ref="B94" r:id="rId77" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/7e56f57e-12e2-49c0-9e51-de68fe9cf789" display="#1 - SIS Acquisition - 2025 AUG" xr:uid="{646A26CD-0D28-4643-9A18-7C11B5F2A6A6}"/>
+    <hyperlink ref="B96" r:id="rId78" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bca1837c-0f90-4529-9649-68676fad5162" display="#2 - SIS Acquisition - 2025 AUG" xr:uid="{97F55F8E-404D-4975-8457-45A84171A0DA}"/>
+    <hyperlink ref="B97" r:id="rId79" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f089ea09-6c3a-40ce-a12b-446940edf922" display="SIS Acquisition Sept 2025 - Segment 3" xr:uid="{04BC038E-0610-489D-8444-24F059E92866}"/>
+    <hyperlink ref="B99" r:id="rId80" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f089ea09-6c3a-40ce-a12b-446940edf922" display="SIS Acquisition Sept 2025 - Segment 3" xr:uid="{D5044EAD-B4FF-4896-9CE0-207234A2ACF4}"/>
+    <hyperlink ref="B98" r:id="rId81" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f089ea09-6c3a-40ce-a12b-446940edf922" display="SIS Acquisition Sept 2025 - Segment 3" xr:uid="{DE061018-F231-4EA6-B230-C6F38A03B8ED}"/>
+    <hyperlink ref="B101" r:id="rId82" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/92b3dff9-2ac0-41da-8e22-ce0ba4df098d" display="SIS Acquisition Sept 2025 - Segment 4  - Cbus" xr:uid="{90DDD61B-B442-447D-BC3F-2F85AAF8535E}"/>
+    <hyperlink ref="B100" r:id="rId83" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/92b3dff9-2ac0-41da-8e22-ce0ba4df098d" xr:uid="{405A91C1-FFD6-4110-8E98-F2CED007F2C4}"/>
+    <hyperlink ref="T93" r:id="rId84" xr:uid="{46A4C0C5-3DA2-4EDE-9262-78B2CEC51B84}"/>
+    <hyperlink ref="T94" r:id="rId85" xr:uid="{AA5FA10A-8377-4821-89EE-5352A329D287}"/>
+    <hyperlink ref="T95" r:id="rId86" xr:uid="{9AA04B41-F1EE-4344-8658-C5D6B7A1AFEA}"/>
+    <hyperlink ref="T96" r:id="rId87" xr:uid="{C2B27C02-626B-497A-93FB-13BB9D4DBBAC}"/>
+    <hyperlink ref="T99" r:id="rId88" xr:uid="{470E4EA3-F735-46B3-B163-4B6833C6BC1E}"/>
+    <hyperlink ref="T97" r:id="rId89" xr:uid="{747F63F2-3DB0-4754-92D2-72D1A8E78BE2}"/>
+    <hyperlink ref="T98" r:id="rId90" xr:uid="{5F3CB8C3-A80F-4108-86AE-76AA502ED4CE}"/>
+    <hyperlink ref="T100" r:id="rId91" xr:uid="{A4F27734-7717-4BB5-9DD8-C6FA10D03B1E}"/>
+    <hyperlink ref="T101" r:id="rId92" xr:uid="{10110FD1-EBB0-40E1-9BB7-56E1B6C67A71}"/>
+    <hyperlink ref="B130" r:id="rId93" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{7B937800-2778-4DA1-909D-7AA3E2D314AE}"/>
+    <hyperlink ref="B55" r:id="rId94" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{38AC2DFC-38D6-4B1E-8941-C0F91073E1DF}"/>
+    <hyperlink ref="B134" r:id="rId95" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{0EC00125-AD37-4C7E-87D0-E41A772F2C30}"/>
+    <hyperlink ref="B57" r:id="rId96" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/c24482ca-6dff-4676-bc67-415d108359fd" display="Cbus News" xr:uid="{9A26CB6A-49BD-4B31-A6A4-92AF61DD4285}"/>
+    <hyperlink ref="B124" r:id="rId97" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b4838304-27ee-40d6-a2c5-fbe51637f011" display="Cbus News Sep - SIS " xr:uid="{9BB6CB4F-35CC-4CCB-A023-11C2EF4DDE69}"/>
+    <hyperlink ref="B123" r:id="rId98" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b4838304-27ee-40d6-a2c5-fbe51637f011" display="Cbus News Sep - SIS " xr:uid="{0B77C253-E7F7-42DB-81B8-1D54AEBD1DE2}"/>
+    <hyperlink ref="B127" r:id="rId99" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/738d4a66-5e39-4d8d-a98d-63f9d66dd930" display="News Sep" xr:uid="{CA7D616B-F1AE-40D0-8563-BC35B1028440}"/>
+    <hyperlink ref="T130" r:id="rId100" xr:uid="{6CD9C4AC-521A-44D2-ABED-C9ADFE5619F9}"/>
+    <hyperlink ref="T132" r:id="rId101" xr:uid="{DECC8875-831C-48D8-A401-5D8F6D6AA9A9}"/>
+    <hyperlink ref="T131" r:id="rId102" xr:uid="{9694BB1C-6051-4A63-9607-0AFC686FEDAC}"/>
+    <hyperlink ref="T134" r:id="rId103" xr:uid="{2AFB76FF-37CE-4C3B-8875-234DF8BBF9B9}"/>
+    <hyperlink ref="T136" r:id="rId104" xr:uid="{47C5D00B-E958-478C-9509-D0B2CD2EC750}"/>
+    <hyperlink ref="T135" r:id="rId105" xr:uid="{F7CD77B8-5717-48A5-9E25-F0A154195DAE}"/>
+    <hyperlink ref="T124" r:id="rId106" xr:uid="{5870EC70-AFC1-4984-B63C-70E52D1997C7}"/>
+    <hyperlink ref="T123" r:id="rId107" xr:uid="{2FE6564C-E9AF-47B3-BC71-8D3F9604053F}"/>
+    <hyperlink ref="T127" r:id="rId108" xr:uid="{CB253886-C65A-44AD-83AA-4CB9936DC0E9}"/>
+    <hyperlink ref="T142" r:id="rId109" xr:uid="{8FD3C9C1-19DD-4DE4-BFED-40C1EDDB16F1}"/>
+    <hyperlink ref="B126" r:id="rId110" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/283624f3-e567-4929-b8bc-d33a9f46ea1e" xr:uid="{FC91E404-A8D6-4EA7-B93E-83446233E670}"/>
+    <hyperlink ref="T126" r:id="rId111" xr:uid="{27456D55-2F72-404D-9C8B-C854698E9165}"/>
+    <hyperlink ref="B125" r:id="rId112" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6a792d2d-ca50-468a-9456-895d03fadfd6" xr:uid="{D4243DDC-749D-4275-B355-E031B567E956}"/>
+    <hyperlink ref="T125" r:id="rId113" xr:uid="{081DB7BB-6798-4BBA-9CAC-132A641DD637}"/>
+    <hyperlink ref="B128" r:id="rId114" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6e06488a-6cb6-428b-9ed6-c8c73ef8b763" xr:uid="{870C6C52-B6E1-4366-9D24-2C1E9D97B15C}"/>
+    <hyperlink ref="B129" r:id="rId115" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6e06488a-6cb6-428b-9ed6-c8c73ef8b763" xr:uid="{0DBE4AED-79C9-4D1F-B6BF-0DF81DB8A6E6}"/>
+    <hyperlink ref="T128" r:id="rId116" xr:uid="{E438F1A1-1B16-4AA3-9219-689FFA1E87CB}"/>
+    <hyperlink ref="T129" r:id="rId117" xr:uid="{25B0C20B-7FC6-45F5-9CF8-EA12B3A78096}"/>
+    <hyperlink ref="B133" r:id="rId118" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/4a7d9c16-ca7f-44aa-a2ef-4239c50d26cc" display="Cbus Advocacy Research Survey - Reminder" xr:uid="{56014A37-0DA9-4BC2-A690-FC44626B215E}"/>
+    <hyperlink ref="T133" r:id="rId119" xr:uid="{084B1D27-4465-483D-85B0-F28273391DB3}"/>
+    <hyperlink ref="B139" r:id="rId120" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/92edf682-d87c-422d-8e7b-bb7d146dc839" xr:uid="{E6EF1D18-86DA-462F-B890-F8805E20CCE5}"/>
+    <hyperlink ref="T139" r:id="rId121" xr:uid="{20B61D8D-19A7-4A3E-A798-10CEE9AEF74B}"/>
+    <hyperlink ref="B137" r:id="rId122" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bc71c7b3-ef48-4aba-ad95-ac8cb9712109" xr:uid="{A22BAA73-5D18-498B-901E-BDD442AEF8DC}"/>
+    <hyperlink ref="B138" r:id="rId123" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bc71c7b3-ef48-4aba-ad95-ac8cb9712109" xr:uid="{1080EF57-D511-42D8-BBD2-1077C17CE1D8}"/>
+    <hyperlink ref="T138" r:id="rId124" xr:uid="{DC7BC730-9C8E-42AB-B523-E4F558909582}"/>
+    <hyperlink ref="T137" r:id="rId125" xr:uid="{EE104E06-0CE6-4434-87A1-BE63E2EC99FD}"/>
+    <hyperlink ref="B144" r:id="rId126" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/39dddfa5-71d3-4db1-89ec-f3482f49b94b" xr:uid="{40523AEF-4573-476A-BF62-104B9F750959}"/>
+    <hyperlink ref="B143" r:id="rId127" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/39dddfa5-71d3-4db1-89ec-f3482f49b94b" xr:uid="{1CF92908-8F0B-478A-A7E0-2E0D1F9C7B4F}"/>
+    <hyperlink ref="T144" r:id="rId128" xr:uid="{85D8ACF6-EC7B-484B-9BEC-B0E24AEFDE3B}"/>
+    <hyperlink ref="T143" r:id="rId129" xr:uid="{8ADCB61D-1BA4-4E3A-B2B6-624284BAD8AF}"/>
+    <hyperlink ref="B145" r:id="rId130" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" xr:uid="{A11CCE1F-CB08-4EF8-8E6D-31B3422A7288}"/>
+    <hyperlink ref="B146" r:id="rId131" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" xr:uid="{DCE34DA4-0432-4EDF-9782-2526B7BF935B}"/>
+    <hyperlink ref="B152" r:id="rId132" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 57 Years - Automated Sep Report" xr:uid="{1832F64D-AA22-48DF-AC5C-5140E44E7706}"/>
+    <hyperlink ref="B151" r:id="rId133" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 57 Years - Automated Sep Report" xr:uid="{5551D050-087E-4390-B182-1616970EBD76}"/>
+    <hyperlink ref="B150" r:id="rId134" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 57 Years - Automated Sep Report" xr:uid="{E4B7E407-4979-4D35-B801-225F790EB799}"/>
+    <hyperlink ref="B149" r:id="rId135" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{CAAF221F-68B7-4199-A185-2DFB46FF1094}"/>
+    <hyperlink ref="T152" r:id="rId136" xr:uid="{D9BF2647-E109-4CB9-81F1-ECD9D09437EB}"/>
+    <hyperlink ref="T151" r:id="rId137" xr:uid="{2A3BE898-28E3-468E-A841-818E5F0AC324}"/>
+    <hyperlink ref="T149" r:id="rId138" xr:uid="{D1171090-F3DC-47A0-9B84-7511891F333E}"/>
+    <hyperlink ref="T150" r:id="rId139" xr:uid="{1C6F57FC-CDBA-4341-9E63-EE9913F028E3}"/>
+    <hyperlink ref="B141" r:id="rId140" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{E9FC87C5-54F7-4CB8-A7F8-DDFE177EAD5D}"/>
+    <hyperlink ref="B140" r:id="rId141" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{7F2080F1-684A-44B5-AEDD-4D722FE1D052}"/>
+    <hyperlink ref="B64" r:id="rId142" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{EB3AA57A-A898-4CA4-B7CE-499CA3EFE349}"/>
+    <hyperlink ref="B62" r:id="rId143" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{D41E71F9-B333-4537-B969-C54B32BAE73F}"/>
+    <hyperlink ref="B113" r:id="rId144" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{EB538D88-BD66-4D15-8B44-94A62534326E}"/>
+    <hyperlink ref="B111" r:id="rId145" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" display="PYS 9 Months - Automated July Report" xr:uid="{F66AD42F-5AC0-484A-B6EA-FAD1DA7827F8}"/>
+    <hyperlink ref="B56" r:id="rId146" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{42560414-F49E-43C7-8271-AF9D9065FC22}"/>
+    <hyperlink ref="B55" r:id="rId147" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{630C694F-30D3-49D8-901D-9014C09E771E}"/>
+    <hyperlink ref="B108" r:id="rId148" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{4C5DDE7F-9FA5-4B76-A6CD-769F71F5FD65}"/>
+    <hyperlink ref="B106" r:id="rId149" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{B9C8B1AB-780B-4793-9196-135A5E0C864A}"/>
+    <hyperlink ref="B65" r:id="rId150" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{3F5521B6-AE14-4530-8B2D-098986E3A2B6}"/>
+    <hyperlink ref="B63" r:id="rId151" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{9859A856-288D-4DBC-8259-0125513EFDD6}"/>
+    <hyperlink ref="B114" r:id="rId152" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{DB4E5029-79AB-4B71-BB4B-DA93872E2665}"/>
+    <hyperlink ref="B112" r:id="rId153" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" display="PYS 5 Months - Automated July Report" xr:uid="{4EB3C59B-5AB6-4FF8-B394-0FBEACB9DDAE}"/>
+    <hyperlink ref="B23" r:id="rId154" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{8BDBBCFB-BFC4-4713-A665-959D3FD8D405}"/>
+    <hyperlink ref="B69" r:id="rId155" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{A5D81D22-5636-4694-8806-92C57FC44478}"/>
+    <hyperlink ref="B67" r:id="rId156" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{23943098-0279-488F-824B-7FBEBCADBD15}"/>
+    <hyperlink ref="B68" r:id="rId157" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{D5B8960F-D042-464A-9468-EE2A6715192E}"/>
+    <hyperlink ref="B66" r:id="rId158" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{7BF59EAE-4D48-4039-9E0B-0DFB48AB37AF}"/>
+    <hyperlink ref="B118" r:id="rId159" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{2B962197-19D1-46CC-9BAF-5E58E2AB29B2}"/>
+    <hyperlink ref="B116" r:id="rId160" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{EDE737E6-545A-4CDA-A2C9-5AAA815C1912}"/>
+    <hyperlink ref="B117" r:id="rId161" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{5C87BAEB-6361-4F87-84AE-35BB546650AA}"/>
+    <hyperlink ref="B115" r:id="rId162" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" display="Consolidation - 90 days -  Automated July Report" xr:uid="{6DE5DBBD-4BC9-44A4-B8A1-2CF44A270889}"/>
+    <hyperlink ref="B61" r:id="rId163" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 73 yrs - Automated July Report" xr:uid="{0BFB927B-249A-4940-A13D-459D0CEDCFCC}"/>
+    <hyperlink ref="B60" r:id="rId164" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 55 yrs - Automated July Report" xr:uid="{441AFB7D-5AC3-460E-9FDB-A402F12EA1F9}"/>
+    <hyperlink ref="B110" r:id="rId165" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 73 yrs - Automated July Report" xr:uid="{99C1F603-EAF1-42FF-B65D-AA1818836699}"/>
+    <hyperlink ref="B109" r:id="rId166" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 55 yrs - Automated July Report" xr:uid="{FE3BD79E-85F1-491C-8D3E-1034584CB3F9}"/>
+    <hyperlink ref="B58" r:id="rId167" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{FB526AFF-EB93-4185-BEAD-58B030C61417}"/>
+    <hyperlink ref="B57" r:id="rId168" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{1B22B47B-D362-437F-B489-CDB4A84B1907}"/>
+    <hyperlink ref="B59" r:id="rId169" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/89e3bf9a-c9fc-4381-a3e2-79ec60962cf0" display="12 Month Check in - 35+ Rolled in - Automated July Report" xr:uid="{C05B998E-F0FE-496D-B2C8-450D8EB2672F}"/>
+    <hyperlink ref="B107" r:id="rId170" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" display="Beneficiaries [Seg 4 - Lapsed binding] - Automated July Report" xr:uid="{29BA7AE2-D727-48C5-8BB6-F40AEBA48DDC}"/>
+    <hyperlink ref="B129:B132" r:id="rId171" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df53f790-6392-4a01-a73f-f23a41796609" display="PYS 12 Months - Automated July Report" xr:uid="{5A57F3AC-8F37-4AA2-AEC3-D228861D25E1}"/>
+    <hyperlink ref="B52" r:id="rId172" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" display="SPC" xr:uid="{7C1DD57D-0992-4981-92FB-393607C4E760}"/>
+    <hyperlink ref="B103" r:id="rId173" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" display="SPC" xr:uid="{4724CBB6-757A-4570-AC13-3FD363F876BC}"/>
+    <hyperlink ref="B137:B138" r:id="rId174" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" display="Abandoned  Cart MJOL" xr:uid="{89E7B679-7362-475D-98BE-25F1829C350A}"/>
+    <hyperlink ref="B147" r:id="rId175" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/bd610eaf-020d-4ee0-8920-be3e08a37a25" xr:uid="{DEABCB06-B632-461D-84C6-F06A70FA9619}"/>
+    <hyperlink ref="B148" r:id="rId176" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3df19f42-c622-481a-a0cc-b64ea8f94164" display="Cbus - 2025 Statements - SIS" xr:uid="{8C7106E8-B2C7-4073-98E2-6BD22D598D4F}"/>
+    <hyperlink ref="T148" r:id="rId177" xr:uid="{46704411-4366-4503-871A-63C62D6F5CDF}"/>
+    <hyperlink ref="T147" r:id="rId178" xr:uid="{35617BE4-D51B-4C42-BCBC-A3326810417E}"/>
+    <hyperlink ref="B153" r:id="rId179" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df121502-9927-4eed-8a89-998f44dfe2cb" xr:uid="{4C7035C0-55DC-42DB-BC1A-1724968D036A}"/>
+    <hyperlink ref="B154" r:id="rId180" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/df121502-9927-4eed-8a89-998f44dfe2cb" xr:uid="{D51BF1B3-CB4F-4C37-97E4-0E8A747D3371}"/>
+    <hyperlink ref="T153" r:id="rId181" xr:uid="{6D9DC780-9CDA-4D3F-B56F-0677CA3C5FB2}"/>
+    <hyperlink ref="T154" r:id="rId182" xr:uid="{E660BB65-5617-4FC2-B761-2C921DC44FB7}"/>
+    <hyperlink ref="B120" r:id="rId183" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{787E3B42-1A34-460D-BCBD-6D1DEBA1028A}"/>
+    <hyperlink ref="B119" r:id="rId184" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" xr:uid="{CAB5B92A-46CB-4743-B631-1BDD2851A0CE}"/>
+    <hyperlink ref="B71" r:id="rId185" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{95384588-A5DD-422B-8251-86A1E34F35E7}"/>
+    <hyperlink ref="B70" r:id="rId186" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{690ACB40-AD80-4398-88D6-EF31DB93FD07}"/>
+    <hyperlink ref="B25" r:id="rId187" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{ACA5534A-56E5-44DB-8EBF-E9C689DD70E6}"/>
+    <hyperlink ref="B24" r:id="rId188" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8c062c79-30ff-4ef1-80d7-e40490c50fab" display="Data Capture- Accum - [Pre 15 Sept 2025]" xr:uid="{8FEB3484-B05E-47F9-99FD-554CD58C3EA1}"/>
+    <hyperlink ref="B122" r:id="rId189" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" xr:uid="{403A0435-2A6E-4B4F-AB1E-59A9DD3D7421}"/>
+    <hyperlink ref="B121" r:id="rId190" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" xr:uid="{70EDC27F-2DC1-4DB6-8815-947052CC4758}"/>
+    <hyperlink ref="B73" r:id="rId191" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" display="6 Month Tenure [Pre 17 Sep 2025]" xr:uid="{BAACE1B3-18DD-40D4-B9D4-9C9FFC7032EA}"/>
+    <hyperlink ref="B72" r:id="rId192" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" display="6 Month Tenure [Pre 17 Sept 2025]" xr:uid="{90BD2120-2520-423A-878B-E4198EC602E4}"/>
+    <hyperlink ref="B153:B154" r:id="rId193" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6c2633f2-243d-40d9-b2d1-214cd45324a9" display="6 Month Tenure [Pre 17 Sept 2025]" xr:uid="{011C95CE-D787-4DFF-A58A-52BB55F1A47F}"/>
+    <hyperlink ref="B157" r:id="rId194" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{95F5B5C6-E7F9-4F03-BCC3-72C6C47E693A}"/>
+    <hyperlink ref="B158" r:id="rId195" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{0A3ED4AD-923A-41AB-8AA4-552B42BFBC3C}"/>
+    <hyperlink ref="B159" r:id="rId196" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{9CD36ECF-BF41-4F3E-9C75-670618C667D2}"/>
+    <hyperlink ref="B160" r:id="rId197" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{3851E138-F07F-4299-82F1-CDACC7AB2D4F}"/>
+    <hyperlink ref="T157" r:id="rId198" xr:uid="{F2675824-1A9F-49D9-A78F-51A609CB7E9D}"/>
+    <hyperlink ref="T158" r:id="rId199" xr:uid="{76235692-6651-4E03-9AAE-80F4C54EA185}"/>
+    <hyperlink ref="T160" r:id="rId200" xr:uid="{B292C362-9C06-4B60-942C-245AE8714903}"/>
+    <hyperlink ref="T159" r:id="rId201" xr:uid="{EF137438-E2BA-480C-9EEA-2E208B2FF391}"/>
+    <hyperlink ref="B156" r:id="rId202" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{594850D2-A800-4945-A1A3-7601E7DFC5BA}"/>
+    <hyperlink ref="B155" r:id="rId203" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" display="Beneficiaries - Seg 1 -New member -  Automated July" xr:uid="{B56A7C75-F3A7-41B8-AB09-941E011BBE2B}"/>
+    <hyperlink ref="B161" r:id="rId204" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{EC7A412D-E0CD-473A-92EC-8B71EC598FC0}"/>
+    <hyperlink ref="B162" r:id="rId205" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{5B6183F1-E7D9-4E23-8A1E-85D2D04FC441}"/>
+    <hyperlink ref="B163" r:id="rId206" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{B402C10B-4B83-4737-83E5-8CFA813ECEB4}"/>
+    <hyperlink ref="B164" r:id="rId207" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{37A7B1A0-5954-4F69-A396-24AAA969F4E7}"/>
+    <hyperlink ref="B165" r:id="rId208" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{B18BF7CB-5575-459F-973A-30561B8958FE}"/>
+    <hyperlink ref="B166" r:id="rId209" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{9D326E37-133E-4777-A180-AD1C95B3D1D2}"/>
+    <hyperlink ref="B167" r:id="rId210" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{F245AA5F-1AE2-4629-900B-0CB71BF249ED}"/>
+    <hyperlink ref="B168" r:id="rId211" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{D5E69B1E-2DD7-48B4-A931-6A46F1D52FE4}"/>
+    <hyperlink ref="B169" r:id="rId212" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{AE17125C-908A-451D-BAB3-78150075D391}"/>
+    <hyperlink ref="B170" r:id="rId213" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cbafab5a-039f-4e19-b165-5c9aea855168" xr:uid="{FCDBE11B-CC1D-44AE-BAC3-6BF06E4A6EEB}"/>
+    <hyperlink ref="B171" r:id="rId214" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{F6A1F5A1-0BCA-4C33-AB46-BD7106ACD0A6}"/>
+    <hyperlink ref="B172" r:id="rId215" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{5D070645-C605-48A6-B30A-545539E44075}"/>
+    <hyperlink ref="B173" r:id="rId216" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" xr:uid="{3D07B372-B516-4FA3-97CF-D7FA84A3AC31}"/>
+    <hyperlink ref="B176" r:id="rId217" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" xr:uid="{F0EF1DE0-C482-4FE6-A769-98A5CF368ADF}"/>
+    <hyperlink ref="B178" r:id="rId218" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" display="6 Month Tenure [Pre 17 Sep 2025]" xr:uid="{560F601D-574D-4934-AD09-006713AC4CDC}"/>
+    <hyperlink ref="B186" r:id="rId219" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{96C74F20-FE6A-40F8-AA31-5644008F3617}"/>
+    <hyperlink ref="T186" r:id="rId220" xr:uid="{D8F82DA6-CC4A-493E-A6B4-B86927821944}"/>
+    <hyperlink ref="B187" r:id="rId221" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/9efc2441-6827-4717-9013-680afb8db7de" xr:uid="{B1D0FF54-7018-42C6-B8F9-A5E1BF28F722}"/>
+    <hyperlink ref="T187" r:id="rId222" xr:uid="{6AE8FEA1-47CB-4F24-B9A5-5E882E21AC38}"/>
+    <hyperlink ref="B188" r:id="rId223" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{8A9343BC-24AB-4F65-8509-CA061FD69388}"/>
+    <hyperlink ref="T188" r:id="rId224" xr:uid="{93AFC6AB-9BA1-4973-92F3-F790ACDE4D19}"/>
+    <hyperlink ref="B189" r:id="rId225" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/745dc927-64df-462b-8819-760afc248605" xr:uid="{14E99629-55BD-48C9-B1BA-1FDF579A92AE}"/>
+    <hyperlink ref="T189" r:id="rId226" xr:uid="{03849D1B-E17B-4AD6-B577-6CF3F1BBB6CD}"/>
+    <hyperlink ref="B191" r:id="rId227" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b3c83ca1-5def-411e-8a8a-b1fa4230bca9" xr:uid="{212C918E-50B9-4332-B1C2-01AD126D7D41}"/>
+    <hyperlink ref="B190" r:id="rId228" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b3c83ca1-5def-411e-8a8a-b1fa4230bca9" xr:uid="{747F800E-4385-4B16-AF7F-18B7A6E1DCBA}"/>
+    <hyperlink ref="B177" r:id="rId229" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" xr:uid="{D2BB8B2B-A730-4842-96DA-050B58161FA7}"/>
+    <hyperlink ref="B193" r:id="rId230" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/11c7ab80-6498-486d-8799-60566311d059" xr:uid="{D028E486-7C5C-4F19-BC7C-4D0BF4854C81}"/>
+    <hyperlink ref="B194" r:id="rId231" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/11c7ab80-6498-486d-8799-60566311d059" xr:uid="{EC080CCE-4AC3-44C9-846F-24E8A6E373E2}"/>
+    <hyperlink ref="B198" r:id="rId232" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{D18EE3B5-4079-4B25-85C7-EED23D580736}"/>
+    <hyperlink ref="B197" r:id="rId233" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" display="Advice Needs research" xr:uid="{102FCE9B-70AE-41E5-87B2-139F4ABCDDFC}"/>
+    <hyperlink ref="B199" r:id="rId234" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{3FE70EE3-023F-4E4B-BBF2-78E8EA52A0B4}"/>
+    <hyperlink ref="B200" r:id="rId235" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e72ad46a-3745-40ba-a629-d9f53273a656" display="Scam awareness EDM" xr:uid="{8AF7365D-29AF-42A6-B6EF-DE0F6A74D90E}"/>
+    <hyperlink ref="B201" r:id="rId236" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e72ad46a-3745-40ba-a629-d9f53273a656" display="Scam awareness EDM" xr:uid="{810FFCD4-E9A1-4CA2-BE71-0B3F9838A0F3}"/>
+    <hyperlink ref="B180" r:id="rId237" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{EC52EDA4-B983-4691-994A-4372BFCF8AB8}"/>
+    <hyperlink ref="B181" r:id="rId238" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{2F265E0D-9A04-4F85-9612-18A7045D0D63}"/>
+    <hyperlink ref="B182" r:id="rId239" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{72F11345-FB57-4891-AFCB-A7021674E90D}"/>
+    <hyperlink ref="B183" r:id="rId240" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{20208A02-C4B2-4288-907A-1191A7C238BE}"/>
+    <hyperlink ref="B179" r:id="rId241" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/35d680d6-e62b-40a2-98e9-8980addab421" display="6 Month Tenure [Pre 17 Sep 2025]" xr:uid="{AABAB842-6D2C-4F7E-85C6-832CD62AC046}"/>
+    <hyperlink ref="B202" r:id="rId242" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/dd583dec-4a8f-4364-b58b-eeb1bca64b4d" xr:uid="{B7F0A43A-9F04-440F-AD9C-9105037D6F5C}"/>
+    <hyperlink ref="B203" r:id="rId243" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/dd583dec-4a8f-4364-b58b-eeb1bca64b4d" xr:uid="{DD788B99-0528-4A31-9DA2-3F14526C441E}"/>
+    <hyperlink ref="B204" r:id="rId244" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1705c74b-00e3-4f10-ba53-8d31b070761f" xr:uid="{17785F7D-009F-47E5-BBC0-003E27DEA98B}"/>
+    <hyperlink ref="B205" r:id="rId245" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1705c74b-00e3-4f10-ba53-8d31b070761f" xr:uid="{D3C43F25-13E2-464D-BC6A-ACA9A0C7C58D}"/>
+    <hyperlink ref="T206" r:id="rId246" xr:uid="{8BE67F82-F3D7-4965-828D-53844EB241DB}"/>
+    <hyperlink ref="T207" r:id="rId247" xr:uid="{F7ECDDC4-C378-4C02-ADFF-9C619DE281B0}"/>
+    <hyperlink ref="T208" r:id="rId248" xr:uid="{DE67BC14-DC57-4C4C-8FE5-3ACFBDA435C4}"/>
+    <hyperlink ref="T217" r:id="rId249" xr:uid="{C7E19626-02A4-4B0C-B60E-86E179849241}"/>
+    <hyperlink ref="T216" r:id="rId250" xr:uid="{D891EFB4-ACAF-45AA-832E-A8B62891E532}"/>
+    <hyperlink ref="T209" r:id="rId251" xr:uid="{308B7210-80CE-4BFD-9B40-FDB3B1E0E14D}"/>
+    <hyperlink ref="T210" r:id="rId252" xr:uid="{5D44B1DF-075A-4461-BA16-F256BCB5DB2F}"/>
+    <hyperlink ref="T211" r:id="rId253" xr:uid="{AC14882E-C08F-418B-89F1-712D6C01D1EB}"/>
+    <hyperlink ref="T212" r:id="rId254" xr:uid="{D65178F1-7C36-4856-968B-BB7AFA21409D}"/>
+    <hyperlink ref="T213" r:id="rId255" xr:uid="{B27A6DAE-AEF7-4B53-BFDF-7010146F131A}"/>
+    <hyperlink ref="T214" r:id="rId256" xr:uid="{8190AD1D-5D8B-4E66-B390-2F27A170F62F}"/>
+    <hyperlink ref="T215" r:id="rId257" xr:uid="{1A1D7CA3-25FC-465E-8689-45457A25D40D}"/>
+    <hyperlink ref="B218" r:id="rId258" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{E1872C75-D226-47E3-AF54-1A01D18B09E6}"/>
+    <hyperlink ref="B219" r:id="rId259" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d7209149-fde7-4ac2-84e6-07fd80500573" xr:uid="{3461D3D2-9801-47C0-BE04-13C65711D695}"/>
+    <hyperlink ref="B220" r:id="rId260" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{D4B47714-368B-4369-BC6A-CE3BF62714B4}"/>
+    <hyperlink ref="B221" r:id="rId261" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/8358282e-963a-4b3a-95a3-3c1846825c9c" xr:uid="{530F7378-391C-4B8F-ABC0-9D46F6F0F7C4}"/>
+    <hyperlink ref="B222" r:id="rId262" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{05123249-3A00-4E04-9FA3-0FAF2BC645C5}"/>
+    <hyperlink ref="B223" r:id="rId263" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/a7179232-e11e-42a4-af3e-d7e193714354" xr:uid="{9EDD1503-471B-46D8-A716-808692FB771A}"/>
+    <hyperlink ref="B224" r:id="rId264" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{F57197D2-BDF7-4008-AFD0-70B7D9715401}"/>
+    <hyperlink ref="B225" r:id="rId265" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" xr:uid="{9CACDA5D-7A93-4498-910D-CB23E2DD242F}"/>
+    <hyperlink ref="B226" r:id="rId266" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" xr:uid="{9AAA07F3-02AF-4AF9-976C-35C0B3FBDD69}"/>
+    <hyperlink ref="B229" r:id="rId267" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e518a319-9c52-4d1e-8c54-5a5bac7e98c1" xr:uid="{60B4CB47-B5E1-4484-AB18-9847FCCFAFF2}"/>
+    <hyperlink ref="B230" r:id="rId268" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" xr:uid="{95C6780C-2B2D-4C98-8481-E4E825CBE9BF}"/>
+    <hyperlink ref="B231" r:id="rId269" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{0021A7F2-DD1B-4870-9404-16898343915B}"/>
+    <hyperlink ref="B232" r:id="rId270" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{53DF61B3-616E-480C-9213-CCC9AC61DF56}"/>
+    <hyperlink ref="B233" r:id="rId271" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{E79F2A25-E7F2-40DB-926C-4F4EB6753687}"/>
+    <hyperlink ref="B234" r:id="rId272" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{DFEB8853-4230-4E7F-84A7-0B899306326B}"/>
+    <hyperlink ref="B227:B228" r:id="rId273" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e1d432aa-88e8-4c3a-89bb-7cfed646e1be" display="PYS 12 Months" xr:uid="{2704B708-84EA-4C85-8C04-062100C8F184}"/>
+    <hyperlink ref="B235" r:id="rId274" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{4C0A1E69-2558-4BB8-B21B-397325219DC8}"/>
+    <hyperlink ref="B236" r:id="rId275" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{76AAD98C-AAC2-4503-AA34-8B434EE3ED3E}"/>
+    <hyperlink ref="B238" r:id="rId276" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{FC9C2CA8-8ABC-4F1E-BB1E-03A815CF8CD8}"/>
+    <hyperlink ref="B237" r:id="rId277" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{8838D11D-6FBD-48CF-9CA4-EDBB1F82F383}"/>
+    <hyperlink ref="B185" r:id="rId278" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{B7867DAB-269E-4524-91A1-534B6EDD7C51}"/>
+    <hyperlink ref="B184" r:id="rId279" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{9D599D62-17C9-498F-8055-4133593F374D}"/>
+    <hyperlink ref="B239" r:id="rId280" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/854f73d8-aa00-4fe2-9c2e-45bcb54156f4" xr:uid="{C1027C14-56EA-448E-8BAB-C63E09D0C9E4}"/>
+    <hyperlink ref="B240" r:id="rId281" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/854f73d8-aa00-4fe2-9c2e-45bcb54156f4" xr:uid="{384E04F6-4003-476E-B192-E063148EA31B}"/>
+    <hyperlink ref="B242" r:id="rId282" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{02010B3C-9466-465E-936C-9470E6B34533}"/>
+    <hyperlink ref="B241" r:id="rId283" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" display="Advice Needs research" xr:uid="{AE77844B-C2CD-4063-8DD4-6E106784FF21}"/>
+    <hyperlink ref="B243" r:id="rId284" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b02f06c5-9124-4f58-a106-99330e115490" xr:uid="{2E8F6402-4182-4DDE-A83F-CCF9127227F3}"/>
+    <hyperlink ref="B241:B243" r:id="rId285" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/09bbe6ac-c38b-4e06-9ae0-fa2b7779445b" display="Advice Needs research- MEDIA 35s+ Reminder" xr:uid="{B63A33C9-482B-449F-9AF5-9895152EAB9F}"/>
+    <hyperlink ref="B244" r:id="rId286" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/51b42ebc-0a9a-4491-a1fa-669bce1a67e7" display="YC Investment Basics" xr:uid="{47D98467-B2C4-4A72-B0B6-64FB8BC26859}"/>
+    <hyperlink ref="B245:B247" r:id="rId287" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/51b42ebc-0a9a-4491-a1fa-669bce1a67e7" display="YC Investment Basics" xr:uid="{5F39ABA6-87A9-4E9D-A6EE-905C88ABE4DF}"/>
+    <hyperlink ref="T244" r:id="rId288" xr:uid="{18314DDC-5F4F-4BDB-A668-B5872785532C}"/>
+    <hyperlink ref="T245" r:id="rId289" xr:uid="{7BADFD5C-DAEF-4DE1-A527-593BE81D4E72}"/>
+    <hyperlink ref="T246" r:id="rId290" xr:uid="{F7E6F66E-D9EA-4898-900D-5532E4671623}"/>
+    <hyperlink ref="T247" r:id="rId291" xr:uid="{5A74C3FC-5D44-4CFB-89D8-A45337A2B428}"/>
+    <hyperlink ref="B248" r:id="rId292" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3e292887-b584-4bcf-8302-372f4e8f75d2" xr:uid="{F6016358-C5B9-40C3-96F3-C601559DB907}"/>
+    <hyperlink ref="B249" r:id="rId293" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/98bceed7-967d-4787-a4c1-29e5d4f011c6" display="Quarterly Investment Perf Update - HNW" xr:uid="{1A2508D2-E90A-4CBB-8B8C-963174C904B8}"/>
+    <hyperlink ref="B250" r:id="rId294" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/98bceed7-967d-4787-a4c1-29e5d4f011c6" display="Quarterly Investment Perf Update - HNW" xr:uid="{0AA40987-2B11-42F9-81C9-236D7843AC8D}"/>
+    <hyperlink ref="T249" r:id="rId295" xr:uid="{D97EE891-4645-49D2-B25F-26C14EFC3BEF}"/>
+    <hyperlink ref="T250" r:id="rId296" xr:uid="{13D1D080-A49D-42A1-8A13-AC04792EAEEB}"/>
+    <hyperlink ref="B251" r:id="rId297" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b2d213d8-d137-4f0b-bd6c-535471820e6f" xr:uid="{0C3F0A6D-5EE8-4501-803F-ADDCAD0ED220}"/>
+    <hyperlink ref="B252" r:id="rId298" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/b2d213d8-d137-4f0b-bd6c-535471820e6f" xr:uid="{38CF9644-43F9-483B-886E-9A492D9C3A3B}"/>
+    <hyperlink ref="T251" r:id="rId299" xr:uid="{678283B0-C9B8-42D6-88C9-59FCE516EEB7}"/>
+    <hyperlink ref="T252" r:id="rId300" xr:uid="{F2DBCCEF-744E-4DBE-9BC8-6CD22C6569A1}"/>
+    <hyperlink ref="B253" r:id="rId301" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f4685d9b-1aa1-48e0-88a5-676af16225cf" xr:uid="{9AB60A34-75B2-46E6-867A-C6D18F6473D8}"/>
+    <hyperlink ref="B254" r:id="rId302" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/f4685d9b-1aa1-48e0-88a5-676af16225cf" xr:uid="{6EBAF5FD-971F-43EB-BC02-D9DED04180AA}"/>
+    <hyperlink ref="T253" r:id="rId303" xr:uid="{EF9898B8-4752-4803-84B4-723099440F4F}"/>
+    <hyperlink ref="T254" r:id="rId304" xr:uid="{2C97B4E3-E071-4FC9-8214-2E7EFF682463}"/>
+    <hyperlink ref="B255" r:id="rId305" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6a9f570b-c2e8-4903-8f56-8a02b73a7926" xr:uid="{6F27F4B5-83E3-4C53-BCB6-11143FEAB1D0}"/>
+    <hyperlink ref="B256" r:id="rId306" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6a9f570b-c2e8-4903-8f56-8a02b73a7926" display="SEN - Death Benefit Nov 25" xr:uid="{D7AAF38C-5652-4386-8A71-3DA5707467F1}"/>
+    <hyperlink ref="T255" r:id="rId307" xr:uid="{3E8DCB2C-2CBD-444A-AE77-A07E924D1512}"/>
+    <hyperlink ref="T256" r:id="rId308" xr:uid="{9A418F6D-2E11-4129-8625-EBA8CBF24892}"/>
+    <hyperlink ref="T257" r:id="rId309" xr:uid="{8D57081E-13DF-438D-889C-CE6E066BDC9C}"/>
+    <hyperlink ref="B278" r:id="rId310" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{8ADD44E8-6354-42E1-BB12-830FDE27E91D}"/>
+    <hyperlink ref="B277" r:id="rId311" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{38563F74-846E-4FAD-99DB-EB52E1F2AE65}"/>
+    <hyperlink ref="B276" r:id="rId312" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{80F0ADC7-54B7-4261-8899-88744AEFCE9F}"/>
+    <hyperlink ref="B275" r:id="rId313" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{90EA5B2E-0B7B-4C4F-837D-0A6B5A5040E0}"/>
+    <hyperlink ref="T281" r:id="rId314" xr:uid="{6FA4FBEE-9AD9-4F61-8D10-C7C9A74A177F}"/>
+    <hyperlink ref="T280" r:id="rId315" xr:uid="{F6F05B44-6AA2-4B51-A325-43FB7485F862}"/>
+    <hyperlink ref="T279" r:id="rId316" xr:uid="{64F605DE-53A2-4520-9ECB-700F494E4B56}"/>
+    <hyperlink ref="B279" r:id="rId317" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{379C56FA-1D5B-4FA2-A31E-C5973A4CD9BF}"/>
+    <hyperlink ref="T265" r:id="rId318" xr:uid="{45BDE7B1-09B3-46B9-BB72-8C0930A078BF}"/>
+    <hyperlink ref="B271" r:id="rId319" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{89DD9A11-62CB-443C-A2DC-91316A733B75}"/>
+    <hyperlink ref="B272" r:id="rId320" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{0D526AE5-9C92-49CC-841E-35EF62220E24}"/>
+    <hyperlink ref="B270" r:id="rId321" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{DE650C40-D448-4F87-94F1-1AE88176FC1C}"/>
+    <hyperlink ref="B269" r:id="rId322" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{C23CDD79-90A2-4C6B-A3DB-33B6822CF85A}"/>
+    <hyperlink ref="B265:B266" r:id="rId323" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e1d432aa-88e8-4c3a-89bb-7cfed646e1be" display="PYS 12 Months" xr:uid="{56C87BF7-E58B-4910-BAD8-FA2366D4FEE7}"/>
+    <hyperlink ref="B268" r:id="rId324" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" display="Abandoned  Cart MJOL" xr:uid="{37A0CAD7-A271-4EDE-A7CB-3AB9E642CBA2}"/>
+    <hyperlink ref="B267" r:id="rId325" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2a36e6fd-dd95-4f8b-87cb-ee5cbb8d6e73" display="SPC - Unpaid Super (Redundant 20251120) " xr:uid="{B5B1C7D8-8DF9-4D9D-B7AF-ACE3656B9CB3}"/>
+    <hyperlink ref="B264" r:id="rId326" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" display="Beneficiaries [Seg 4 - Lapsed binding] (Stop 22 Dec)" xr:uid="{947451C0-F3E8-410C-B94E-AE666A563C27}"/>
+    <hyperlink ref="B263" r:id="rId327" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 55 yrs (Stop 22 Dec)" xr:uid="{884D2A54-DC16-4160-8FE3-AFED9BE7722A}"/>
+    <hyperlink ref="B262" r:id="rId328" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 73 yrs - (Stop 22 Dec)" xr:uid="{C628F592-2342-4EE7-AFD5-99A84D5762D5}"/>
+    <hyperlink ref="T261" r:id="rId329" xr:uid="{D5762008-1984-4804-BF9A-2485573B0A1D}"/>
+    <hyperlink ref="T260" r:id="rId330" xr:uid="{8633495D-53BC-4CCB-987E-FF235604B280}"/>
+    <hyperlink ref="T259" r:id="rId331" xr:uid="{54B4B942-FEEB-476D-93A8-2D81479DC092}"/>
+    <hyperlink ref="T258" r:id="rId332" xr:uid="{D1B9CD42-A935-4D74-9DB5-F2F2D2E0CAC4}"/>
+    <hyperlink ref="B261" r:id="rId333" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{B9DD3996-A656-413E-A205-65D707DAB485}"/>
+    <hyperlink ref="B260" r:id="rId334" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{1A8763F8-E195-441A-A099-16AA0DDC0D04}"/>
     <hyperlink ref="B259" r:id="rId335" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{D864079F-919D-4730-9C4E-9BFDD5A3FCCF}"/>
-    <hyperlink ref="B260" r:id="rId336" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{1A8763F8-E195-441A-A099-16AA0DDC0D04}"/>
-    <hyperlink ref="B261" r:id="rId337" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{B9DD3996-A656-413E-A205-65D707DAB485}"/>
-    <hyperlink ref="T258" r:id="rId338" xr:uid="{D1B9CD42-A935-4D74-9DB5-F2F2D2E0CAC4}"/>
-    <hyperlink ref="T259" r:id="rId339" xr:uid="{54B4B942-FEEB-476D-93A8-2D81479DC092}"/>
-    <hyperlink ref="T260" r:id="rId340" xr:uid="{8633495D-53BC-4CCB-987E-FF235604B280}"/>
-    <hyperlink ref="T261" r:id="rId341" xr:uid="{D5762008-1984-4804-BF9A-2485573B0A1D}"/>
-    <hyperlink ref="B262" r:id="rId342" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 73 yrs - (Stop 22 Dec)" xr:uid="{C628F592-2342-4EE7-AFD5-99A84D5762D5}"/>
-    <hyperlink ref="B263" r:id="rId343" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/ae73d654-f7fb-4218-a985-79965ed53f32" display="Downsizer - 55 yrs (Stop 22 Dec)" xr:uid="{884D2A54-DC16-4160-8FE3-AFED9BE7722A}"/>
-    <hyperlink ref="B264" r:id="rId344" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/785d6f2f-8292-422a-9833-2d2802ca7fa1" display="Beneficiaries [Seg 4 - Lapsed binding] (Stop 22 Dec)" xr:uid="{947451C0-F3E8-410C-B94E-AE666A563C27}"/>
-    <hyperlink ref="B267" r:id="rId345" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/2a36e6fd-dd95-4f8b-87cb-ee5cbb8d6e73" display="SPC - Unpaid Super (Redundant 20251120) " xr:uid="{B5B1C7D8-8DF9-4D9D-B7AF-ACE3656B9CB3}"/>
-    <hyperlink ref="B268" r:id="rId346" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/1428586f-9ad2-4562-8874-284efe3c0c8d" display="Abandoned  Cart MJOL" xr:uid="{37A0CAD7-A271-4EDE-A7CB-3AB9E642CBA2}"/>
-    <hyperlink ref="B265:B266" r:id="rId347" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/e1d432aa-88e8-4c3a-89bb-7cfed646e1be" display="PYS 12 Months" xr:uid="{56C87BF7-E58B-4910-BAD8-FA2366D4FEE7}"/>
-    <hyperlink ref="B269" r:id="rId348" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{C23CDD79-90A2-4C6B-A3DB-33B6822CF85A}"/>
-    <hyperlink ref="B270" r:id="rId349" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/6b33825c-fbb5-4f47-b564-a293510bba4f" xr:uid="{DE650C40-D448-4F87-94F1-1AE88176FC1C}"/>
-    <hyperlink ref="B272" r:id="rId350" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{0D526AE5-9C92-49CC-841E-35EF62220E24}"/>
-    <hyperlink ref="B271" r:id="rId351" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/23e4f381-4c2b-457e-b600-83d098bf6354" display="Data Capture [Sept 2025] - Automated Sep Report" xr:uid="{89DD9A11-62CB-443C-A2DC-91316A733B75}"/>
-    <hyperlink ref="T265" r:id="rId352" xr:uid="{45BDE7B1-09B3-46B9-BB72-8C0930A078BF}"/>
-    <hyperlink ref="B273" r:id="rId353" location="/@cbus/sname:prod/journey-optimizer/journey/report/" xr:uid="{379C56FA-1D5B-4FA2-A31E-C5973A4CD9BF}"/>
-    <hyperlink ref="T273" r:id="rId354" xr:uid="{64F605DE-53A2-4520-9ECB-700F494E4B56}"/>
-    <hyperlink ref="T274" r:id="rId355" xr:uid="{F6F05B44-6AA2-4B51-A325-43FB7485F862}"/>
-    <hyperlink ref="T275" r:id="rId356" xr:uid="{6FA4FBEE-9AD9-4F61-8D10-C7C9A74A177F}"/>
-    <hyperlink ref="B276" r:id="rId357" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 68 Years [Pre 25 Sep 2025]" xr:uid="{90EA5B2E-0B7B-4C4F-837D-0A6B5A5040E0}"/>
-    <hyperlink ref="B277" r:id="rId358" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 67 Years Pre 25 Sep 2025]" xr:uid="{80F0ADC7-54B7-4261-8899-88744AEFCE9F}"/>
-    <hyperlink ref="B278" r:id="rId359" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" display="Age Pension - 66 Years [Pre 25 Sep 2025]" xr:uid="{38563F74-846E-4FAD-99DB-EB52E1F2AE65}"/>
-    <hyperlink ref="B279" r:id="rId360" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/3cbde0fd-ec21-4c5d-bbac-0292e906b9e5" xr:uid="{8ADD44E8-6354-42E1-BB12-830FDE27E91D}"/>
+    <hyperlink ref="B258" r:id="rId336" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/cb50294d-186e-4efb-a08c-5bd962403459" display="Cbus - Accessing Super &amp; SIS " xr:uid="{A194A329-BFAE-4C41-A6E8-5281732B1448}"/>
+    <hyperlink ref="B273" r:id="rId337" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d21ac559-604d-446d-8bf4-e1c8c6ea0563" display="PYS 9 Months (20-Nov End)" xr:uid="{966A009C-A803-4448-A826-5E8A67F36729}"/>
+    <hyperlink ref="B274" r:id="rId338" location="/@cbus/sname:prod/journey-optimizer/journey/report/#/workspace/template/ajo-journey/d21ac559-604d-446d-8bf4-e1c8c6ea0563" xr:uid="{33E021F7-D5B9-4897-B8F5-23289ADAE09A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId361"/>
+  <legacyDrawing r:id="rId339"/>
   <tableParts count="1">
-    <tablePart r:id="rId362"/>
+    <tablePart r:id="rId340"/>
   </tableParts>
 </worksheet>
 </file>
@@ -22640,44 +22755,44 @@
   <sheetData>
     <row r="1" spans="1:2" s="120" customFormat="1">
       <c r="A1" s="121" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B1" s="119"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="122" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B2" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!L:L))</f>
-        <v>64.699678073787155</v>
+        <v>64.700957569649518</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="122" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B3" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!M:M))</f>
-        <v>6.4993639288398866</v>
+        <v>6.5059975840938948</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="122" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B4" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!N:N))</f>
-        <v>9.9519729877069345</v>
+        <v>9.9619283286570326</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="122" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B5" s="118">
         <f>SUM(AVERAGE('FY-ajo-report'!K:K))</f>
-        <v>0.15005606257382187</v>
+        <v>0.14970090818515555</v>
       </c>
     </row>
   </sheetData>
@@ -22686,19 +22801,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005CAB1339F159CD428AD0F5BA99C368F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3c12e32d35f281fc2cfbff59ce227b1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0eeac73-9918-465e-bdd8-785547fbc2d9" xmlns:ns3="d777fa6b-bca0-4864-8d50-ac77b155e846" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8cccd8974b01cfe5577657fdcd6042cb" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005CAB1339F159CD428AD0F5BA99C368F2" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be1e989bef91ac63627d5ae0da3c3c75">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0eeac73-9918-465e-bdd8-785547fbc2d9" xmlns:ns3="d777fa6b-bca0-4864-8d50-ac77b155e846" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9915e4f6c3f750f88ff3d934d8bc3e74" ns2:_="" ns3:_="">
     <xsd:import namespace="c0eeac73-9918-465e-bdd8-785547fbc2d9"/>
     <xsd:import namespace="d777fa6b-bca0-4864-8d50-ac77b155e846"/>
     <xsd:element name="properties">
@@ -22932,24 +23045,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0ECD7C-9783-4AF2-B19D-668092346D66}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EBF9AAC-F6EE-4F9D-A850-BD5FE7C93CA6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41A8F991-C20E-41DA-86BA-BB1F28819AFA}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0ECD7C-9783-4AF2-B19D-668092346D66}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
add PYS 9 MS image
</commit_message>
<xml_diff>
--- a/pages/dashboard/data/email-report-fy26.xlsx
+++ b/pages/dashboard/data/email-report-fy26.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cbussuper.sharepoint.com/sites/MarketingTechTeam/Shared Documents/Reporting/FY26/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CCC12F6-761E-4E67-A1B9-E0A2F4641D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEF3BAE9-89FD-4853-90C8-04C470E8B57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{2AF7D318-117B-4C45-A242-FA29CA5E08DD}"/>
   </bookViews>
@@ -1575,7 +1575,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" indent="1"/>
@@ -1914,12 +1914,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3029,8 +3023,8 @@
   <dimension ref="A1:T281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A275" sqref="A275:XFD275"/>
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A222" sqref="A222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="32.1" customHeight="1"/>
@@ -4090,7 +4084,7 @@
     </row>
     <row r="16" spans="1:20" ht="32.1" customHeight="1">
       <c r="A16" s="74">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="B16" s="104" t="s">
         <v>39</v>
@@ -7296,7 +7290,7 @@
     </row>
     <row r="62" spans="1:20" ht="32.1" customHeight="1">
       <c r="A62" s="75">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="B62" s="104" t="s">
         <v>39</v>
@@ -10729,7 +10723,7 @@
     </row>
     <row r="111" spans="1:20" ht="32.1" customHeight="1">
       <c r="A111" s="75">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="B111" s="106" t="s">
         <v>39</v>
@@ -14430,7 +14424,7 @@
     </row>
     <row r="164" spans="1:20" ht="32.1" customHeight="1">
       <c r="A164" s="81">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="B164" s="108" t="s">
         <v>39</v>
@@ -18247,7 +18241,7 @@
     </row>
     <row r="221" spans="1:20" ht="32.1" customHeight="1">
       <c r="A221" s="81">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="B221" s="108" t="s">
         <v>235</v>
@@ -21818,7 +21812,7 @@
     </row>
     <row r="274" spans="1:20" ht="32.1" customHeight="1">
       <c r="A274" s="81">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="B274" s="84" t="s">
         <v>282</v>
@@ -22197,16 +22191,16 @@
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
         <v>🔴</v>
       </c>
-      <c r="Q279" s="125">
+      <c r="Q279" s="14">
         <v>73.2</v>
       </c>
-      <c r="R279" s="126">
+      <c r="R279" s="16">
         <v>16.100000000000001</v>
       </c>
-      <c r="S279" s="126">
+      <c r="S279" s="16">
         <v>10.7</v>
       </c>
-      <c r="T279" s="127" t="s">
+      <c r="T279" s="125" t="s">
         <v>288</v>
       </c>
     </row>
@@ -22268,16 +22262,16 @@
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
         <v>🟡</v>
       </c>
-      <c r="Q280" s="125">
+      <c r="Q280" s="14">
         <v>40</v>
       </c>
-      <c r="R280" s="126">
+      <c r="R280" s="16">
         <v>26.7</v>
       </c>
-      <c r="S280" s="126">
+      <c r="S280" s="16">
         <v>33.299999999999997</v>
       </c>
-      <c r="T280" s="127" t="s">
+      <c r="T280" s="125" t="s">
         <v>290</v>
       </c>
     </row>
@@ -22339,16 +22333,16 @@
         <f>IF(Table1[[#This Row],[Engagement Score]]&lt;30,"🔴",IF(Table1[[#This Row],[Engagement Score]]&lt;40,"🟡","🟢"))</f>
         <v>🟡</v>
       </c>
-      <c r="Q281" s="125">
+      <c r="Q281" s="14">
         <v>77.2</v>
       </c>
-      <c r="R281" s="126">
+      <c r="R281" s="16">
         <v>16.399999999999999</v>
       </c>
-      <c r="S281" s="126">
+      <c r="S281" s="16">
         <v>6.4</v>
       </c>
-      <c r="T281" s="127" t="s">
+      <c r="T281" s="125" t="s">
         <v>292</v>
       </c>
     </row>
@@ -22801,12 +22795,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23045,18 +23041,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d777fa6b-bca0-4864-8d50-ac77b155e846" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0eeac73-9918-465e-bdd8-785547fbc2d9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0ECD7C-9783-4AF2-B19D-668092346D66}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23064,7 +23058,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BB0AA99-F2C0-47AC-BEFF-11024E9EC09D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE0ECD7C-9783-4AF2-B19D-668092346D66}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>